<commit_message>
change operator ">" to ">="
</commit_message>
<xml_diff>
--- a/Article_17_EU-2022.xlsx
+++ b/Article_17_EU-2022.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B59F21D-E1EA-404C-8CFB-5C195DEC5A02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B58D88DA-0916-4EC6-B0B0-76688B7752C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1313" yWindow="907" windowWidth="14614" windowHeight="10053" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="3135" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="article_17_synthesis_table" sheetId="1" r:id="rId1"/>
@@ -73,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4113" uniqueCount="395">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4109" uniqueCount="391">
   <si>
     <t>Forecast for investments needs by national authorities</t>
   </si>
@@ -1459,9 +1459,6 @@
     <t>2026-2031</t>
   </si>
   <si>
-    <t>2027-2029</t>
-  </si>
-  <si>
     <t>2025-2029</t>
   </si>
   <si>
@@ -1484,9 +1481,6 @@
   </si>
   <si>
     <t>2030-2030</t>
-  </si>
-  <si>
-    <t>2025-2033</t>
   </si>
   <si>
     <t>2028-2029</t>
@@ -1531,28 +1525,10 @@
     <t>2024-2030</t>
   </si>
   <si>
-    <t>2024-2031</t>
-  </si>
-  <si>
-    <t>2024-2036</t>
-  </si>
-  <si>
-    <t>2024-2034</t>
-  </si>
-  <si>
     <t>2025 - 2032</t>
   </si>
   <si>
-    <t>2024 - 2030</t>
-  </si>
-  <si>
     <t>2030 - 2030</t>
-  </si>
-  <si>
-    <t>2024 - 2033</t>
-  </si>
-  <si>
-    <t>2024 - 2027</t>
   </si>
   <si>
     <t>2027 - 2028</t>
@@ -1561,31 +1537,43 @@
     <t>2026 - 2026</t>
   </si>
   <si>
-    <t>2024 - 2031</t>
-  </si>
-  <si>
     <t>2026 - 2030</t>
   </si>
   <si>
     <t>2024 - 2032</t>
   </si>
   <si>
-    <t>2024 - 2025</t>
+    <t>3296.5 (+IAS 523)</t>
   </si>
   <si>
-    <t>2024 - 2036</t>
+    <t>2023-2036</t>
   </si>
   <si>
-    <t>2024 - 2035</t>
+    <t>2023-2034</t>
   </si>
   <si>
-    <t>2024 - 2034</t>
+    <t>2023 - 2033</t>
   </si>
   <si>
-    <t>2024 - 2028</t>
+    <t>2023 - 2027</t>
   </si>
   <si>
-    <t>3296.5 (+IAS 523)</t>
+    <t>2023 - 2031</t>
+  </si>
+  <si>
+    <t>2023 - 2025</t>
+  </si>
+  <si>
+    <t>2023 - 2036</t>
+  </si>
+  <si>
+    <t>2023 - 2035</t>
+  </si>
+  <si>
+    <t>2023 - 2034</t>
+  </si>
+  <si>
+    <t>2023 - 2028</t>
   </si>
 </sst>
 </file>
@@ -1863,7 +1851,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -2066,6 +2054,108 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="22"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="22"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="22"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="22"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -2081,7 +2171,7 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="127">
+  <cellXfs count="180">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2345,6 +2435,152 @@
     <xf numFmtId="3" fontId="4" fillId="16" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="10" fontId="9" fillId="9" borderId="1" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="6" borderId="9" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="6" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="9" fillId="9" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="9" fillId="9" borderId="9" xfId="9" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="4" fillId="6" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="6" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="8" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="16" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="6" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="9" fillId="9" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="9" fillId="9" borderId="12" xfId="9" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="4" fillId="6" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="6" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="8" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="16" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="4" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="4" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="6" borderId="21" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="6" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="9" fillId="9" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="9" fillId="9" borderId="21" xfId="9" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="4" fillId="6" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="6" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="8" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="16" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -2420,7 +2656,6 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="10" fontId="9" fillId="9" borderId="1" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="12">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2720,9 +2955,9 @@
   <sheetPr codeName="Feuil1"/>
   <dimension ref="A1:HC56"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B45" sqref="B45:C45"/>
+    <sheetView tabSelected="1" topLeftCell="X1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AA23" sqref="AA23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -2739,7 +2974,8 @@
     <col min="20" max="23" width="11.87890625" customWidth="1"/>
     <col min="24" max="24" width="14.52734375" customWidth="1"/>
     <col min="25" max="25" width="18.52734375" customWidth="1"/>
-    <col min="26" max="27" width="13.234375" customWidth="1"/>
+    <col min="26" max="26" width="13.234375" customWidth="1"/>
+    <col min="27" max="27" width="13.234375" style="142" customWidth="1"/>
     <col min="28" max="39" width="11.87890625" customWidth="1"/>
     <col min="40" max="40" width="15.64453125" customWidth="1"/>
     <col min="41" max="43" width="18.1171875" customWidth="1"/>
@@ -2781,172 +3017,172 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:113" s="88" customFormat="1" ht="24.45" customHeight="1" x14ac:dyDescent="0.7">
-      <c r="D1" s="101" t="s">
+      <c r="D1" s="155" t="s">
         <v>41</v>
       </c>
-      <c r="E1" s="102"/>
-      <c r="F1" s="102"/>
-      <c r="G1" s="103"/>
-      <c r="H1" s="101" t="s">
+      <c r="E1" s="156"/>
+      <c r="F1" s="156"/>
+      <c r="G1" s="157"/>
+      <c r="H1" s="155" t="s">
         <v>42</v>
       </c>
-      <c r="I1" s="102"/>
-      <c r="J1" s="102"/>
-      <c r="K1" s="103"/>
-      <c r="L1" s="101" t="s">
+      <c r="I1" s="156"/>
+      <c r="J1" s="156"/>
+      <c r="K1" s="157"/>
+      <c r="L1" s="155" t="s">
         <v>43</v>
       </c>
-      <c r="M1" s="102"/>
-      <c r="N1" s="102"/>
-      <c r="O1" s="103"/>
-      <c r="P1" s="101" t="s">
+      <c r="M1" s="156"/>
+      <c r="N1" s="156"/>
+      <c r="O1" s="157"/>
+      <c r="P1" s="155" t="s">
         <v>44</v>
       </c>
-      <c r="Q1" s="102"/>
-      <c r="R1" s="102"/>
-      <c r="S1" s="103"/>
-      <c r="T1" s="101" t="s">
+      <c r="Q1" s="156"/>
+      <c r="R1" s="156"/>
+      <c r="S1" s="157"/>
+      <c r="T1" s="155" t="s">
         <v>45</v>
       </c>
-      <c r="U1" s="102"/>
-      <c r="V1" s="102"/>
-      <c r="W1" s="103"/>
-      <c r="X1" s="101" t="s">
+      <c r="U1" s="156"/>
+      <c r="V1" s="156"/>
+      <c r="W1" s="157"/>
+      <c r="X1" s="155" t="s">
         <v>46</v>
       </c>
-      <c r="Y1" s="102"/>
-      <c r="Z1" s="102"/>
-      <c r="AA1" s="103"/>
-      <c r="AB1" s="101" t="s">
+      <c r="Y1" s="156"/>
+      <c r="Z1" s="156"/>
+      <c r="AA1" s="157"/>
+      <c r="AB1" s="155" t="s">
         <v>47</v>
       </c>
-      <c r="AC1" s="102"/>
-      <c r="AD1" s="102"/>
-      <c r="AE1" s="103"/>
-      <c r="AF1" s="101" t="s">
+      <c r="AC1" s="156"/>
+      <c r="AD1" s="156"/>
+      <c r="AE1" s="157"/>
+      <c r="AF1" s="155" t="s">
         <v>48</v>
       </c>
-      <c r="AG1" s="102"/>
-      <c r="AH1" s="102"/>
-      <c r="AI1" s="103"/>
-      <c r="AJ1" s="101" t="s">
+      <c r="AG1" s="156"/>
+      <c r="AH1" s="156"/>
+      <c r="AI1" s="157"/>
+      <c r="AJ1" s="155" t="s">
         <v>49</v>
       </c>
-      <c r="AK1" s="102"/>
-      <c r="AL1" s="102"/>
-      <c r="AM1" s="103"/>
-      <c r="AN1" s="101" t="s">
+      <c r="AK1" s="156"/>
+      <c r="AL1" s="156"/>
+      <c r="AM1" s="157"/>
+      <c r="AN1" s="155" t="s">
         <v>50</v>
       </c>
-      <c r="AO1" s="102"/>
-      <c r="AP1" s="102"/>
-      <c r="AQ1" s="103"/>
-      <c r="AR1" s="101" t="s">
+      <c r="AO1" s="156"/>
+      <c r="AP1" s="156"/>
+      <c r="AQ1" s="157"/>
+      <c r="AR1" s="155" t="s">
         <v>51</v>
       </c>
-      <c r="AS1" s="102"/>
-      <c r="AT1" s="102"/>
-      <c r="AU1" s="103"/>
-      <c r="AV1" s="101" t="s">
+      <c r="AS1" s="156"/>
+      <c r="AT1" s="156"/>
+      <c r="AU1" s="157"/>
+      <c r="AV1" s="155" t="s">
         <v>52</v>
       </c>
-      <c r="AW1" s="102"/>
-      <c r="AX1" s="102"/>
-      <c r="AY1" s="103"/>
-      <c r="AZ1" s="101" t="s">
+      <c r="AW1" s="156"/>
+      <c r="AX1" s="156"/>
+      <c r="AY1" s="157"/>
+      <c r="AZ1" s="155" t="s">
         <v>53</v>
       </c>
-      <c r="BA1" s="102"/>
-      <c r="BB1" s="102"/>
-      <c r="BC1" s="103"/>
-      <c r="BD1" s="101" t="s">
+      <c r="BA1" s="156"/>
+      <c r="BB1" s="156"/>
+      <c r="BC1" s="157"/>
+      <c r="BD1" s="155" t="s">
         <v>54</v>
       </c>
-      <c r="BE1" s="102"/>
-      <c r="BF1" s="102"/>
-      <c r="BG1" s="103"/>
-      <c r="BH1" s="101" t="s">
+      <c r="BE1" s="156"/>
+      <c r="BF1" s="156"/>
+      <c r="BG1" s="157"/>
+      <c r="BH1" s="155" t="s">
         <v>55</v>
       </c>
-      <c r="BI1" s="102"/>
-      <c r="BJ1" s="102"/>
-      <c r="BK1" s="103"/>
-      <c r="BL1" s="101" t="s">
+      <c r="BI1" s="156"/>
+      <c r="BJ1" s="156"/>
+      <c r="BK1" s="157"/>
+      <c r="BL1" s="155" t="s">
         <v>56</v>
       </c>
-      <c r="BM1" s="102"/>
-      <c r="BN1" s="102"/>
-      <c r="BO1" s="103"/>
-      <c r="BP1" s="101" t="s">
+      <c r="BM1" s="156"/>
+      <c r="BN1" s="156"/>
+      <c r="BO1" s="157"/>
+      <c r="BP1" s="155" t="s">
         <v>57</v>
       </c>
-      <c r="BQ1" s="102"/>
-      <c r="BR1" s="102"/>
-      <c r="BS1" s="103"/>
-      <c r="BT1" s="101" t="s">
+      <c r="BQ1" s="156"/>
+      <c r="BR1" s="156"/>
+      <c r="BS1" s="157"/>
+      <c r="BT1" s="155" t="s">
         <v>58</v>
       </c>
-      <c r="BU1" s="102"/>
-      <c r="BV1" s="102"/>
-      <c r="BW1" s="103"/>
-      <c r="BX1" s="101" t="s">
+      <c r="BU1" s="156"/>
+      <c r="BV1" s="156"/>
+      <c r="BW1" s="157"/>
+      <c r="BX1" s="155" t="s">
         <v>59</v>
       </c>
-      <c r="BY1" s="102"/>
-      <c r="BZ1" s="102"/>
-      <c r="CA1" s="103"/>
-      <c r="CB1" s="101" t="s">
+      <c r="BY1" s="156"/>
+      <c r="BZ1" s="156"/>
+      <c r="CA1" s="157"/>
+      <c r="CB1" s="155" t="s">
         <v>60</v>
       </c>
-      <c r="CC1" s="102"/>
-      <c r="CD1" s="102"/>
-      <c r="CE1" s="103"/>
-      <c r="CF1" s="101" t="s">
+      <c r="CC1" s="156"/>
+      <c r="CD1" s="156"/>
+      <c r="CE1" s="157"/>
+      <c r="CF1" s="155" t="s">
         <v>61</v>
       </c>
-      <c r="CG1" s="102"/>
-      <c r="CH1" s="102"/>
-      <c r="CI1" s="103"/>
-      <c r="CJ1" s="101" t="s">
+      <c r="CG1" s="156"/>
+      <c r="CH1" s="156"/>
+      <c r="CI1" s="157"/>
+      <c r="CJ1" s="155" t="s">
         <v>62</v>
       </c>
-      <c r="CK1" s="102"/>
-      <c r="CL1" s="102"/>
-      <c r="CM1" s="103"/>
-      <c r="CN1" s="101" t="s">
+      <c r="CK1" s="156"/>
+      <c r="CL1" s="156"/>
+      <c r="CM1" s="157"/>
+      <c r="CN1" s="155" t="s">
         <v>63</v>
       </c>
-      <c r="CO1" s="102"/>
-      <c r="CP1" s="102"/>
-      <c r="CQ1" s="103"/>
-      <c r="CR1" s="101" t="s">
+      <c r="CO1" s="156"/>
+      <c r="CP1" s="156"/>
+      <c r="CQ1" s="157"/>
+      <c r="CR1" s="155" t="s">
         <v>64</v>
       </c>
-      <c r="CS1" s="102"/>
-      <c r="CT1" s="102"/>
-      <c r="CU1" s="103"/>
-      <c r="CV1" s="101" t="s">
+      <c r="CS1" s="156"/>
+      <c r="CT1" s="156"/>
+      <c r="CU1" s="157"/>
+      <c r="CV1" s="155" t="s">
         <v>65</v>
       </c>
-      <c r="CW1" s="102"/>
-      <c r="CX1" s="102"/>
-      <c r="CY1" s="103"/>
-      <c r="CZ1" s="101" t="s">
+      <c r="CW1" s="156"/>
+      <c r="CX1" s="156"/>
+      <c r="CY1" s="157"/>
+      <c r="CZ1" s="155" t="s">
         <v>66</v>
       </c>
-      <c r="DA1" s="102"/>
-      <c r="DB1" s="102"/>
-      <c r="DC1" s="103"/>
-      <c r="DD1" s="101" t="s">
+      <c r="DA1" s="156"/>
+      <c r="DB1" s="156"/>
+      <c r="DC1" s="157"/>
+      <c r="DD1" s="155" t="s">
         <v>67</v>
       </c>
-      <c r="DE1" s="102"/>
-      <c r="DF1" s="102"/>
-      <c r="DG1" s="103"/>
-      <c r="DH1" s="101" t="s">
+      <c r="DE1" s="156"/>
+      <c r="DF1" s="156"/>
+      <c r="DG1" s="157"/>
+      <c r="DH1" s="155" t="s">
         <v>68</v>
       </c>
-      <c r="DI1" s="103"/>
+      <c r="DI1" s="157"/>
     </row>
     <row r="2" spans="2:113" s="90" customFormat="1" ht="16.7" customHeight="1" x14ac:dyDescent="0.5">
       <c r="D2" s="91" t="s">
@@ -3018,10 +3254,10 @@
       <c r="Z2" s="91" t="s">
         <v>74</v>
       </c>
-      <c r="AA2" s="91" t="s">
+      <c r="AA2" s="136" t="s">
         <v>74</v>
       </c>
-      <c r="AB2" s="91" t="s">
+      <c r="AB2" s="119" t="s">
         <v>75</v>
       </c>
       <c r="AC2" s="91" t="s">
@@ -3281,10 +3517,10 @@
       </c>
     </row>
     <row r="3" spans="2:113" s="93" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="B3" s="106" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="106"/>
+      <c r="B3" s="160" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="160"/>
       <c r="D3" s="92">
         <v>2016</v>
       </c>
@@ -3351,13 +3587,13 @@
       <c r="Y3" s="92">
         <v>2018</v>
       </c>
-      <c r="Z3" s="92">
+      <c r="Z3" s="102">
         <v>2020</v>
       </c>
-      <c r="AA3" s="92">
+      <c r="AA3" s="137">
         <v>2022</v>
       </c>
-      <c r="AB3" s="92">
+      <c r="AB3" s="120">
         <v>2016</v>
       </c>
       <c r="AC3" s="92">
@@ -3643,9 +3879,9 @@
       <c r="W4" s="6"/>
       <c r="X4" s="6"/>
       <c r="Y4" s="6"/>
-      <c r="Z4" s="6"/>
-      <c r="AA4" s="6"/>
-      <c r="AB4" s="6"/>
+      <c r="Z4" s="103"/>
+      <c r="AA4" s="138"/>
+      <c r="AB4" s="121"/>
       <c r="AC4" s="6"/>
       <c r="AD4" s="6"/>
       <c r="AE4" s="6"/>
@@ -3759,9 +3995,9 @@
       <c r="W5" s="7"/>
       <c r="X5" s="7"/>
       <c r="Y5" s="7"/>
-      <c r="Z5" s="7"/>
-      <c r="AA5" s="7"/>
-      <c r="AB5" s="7"/>
+      <c r="Z5" s="104"/>
+      <c r="AA5" s="139"/>
+      <c r="AB5" s="122"/>
       <c r="AC5" s="7"/>
       <c r="AD5" s="7"/>
       <c r="AE5" s="7"/>
@@ -3849,7 +4085,7 @@
       <c r="DI5" s="7"/>
     </row>
     <row r="6" spans="2:113" ht="22.85" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B6" s="104" t="s">
+      <c r="B6" s="158" t="s">
         <v>3</v>
       </c>
       <c r="C6" s="8" t="s">
@@ -3913,7 +4149,7 @@
         <v>311.6832</v>
       </c>
       <c r="W6" s="16">
-        <v>458.75907100000001</v>
+        <v>476.96700499999997</v>
       </c>
       <c r="X6" s="16">
         <v>0</v>
@@ -3921,13 +4157,13 @@
       <c r="Y6" s="17" t="s">
         <v>137</v>
       </c>
-      <c r="Z6" s="17" t="s">
-        <v>137</v>
-      </c>
-      <c r="AA6" s="17" t="s">
-        <v>137</v>
-      </c>
-      <c r="AB6" s="16" t="s">
+      <c r="Z6" s="105" t="s">
+        <v>137</v>
+      </c>
+      <c r="AA6" s="140" t="s">
+        <v>137</v>
+      </c>
+      <c r="AB6" s="123" t="s">
         <v>137</v>
       </c>
       <c r="AC6" s="17" t="s">
@@ -3997,7 +4233,7 @@
         <v>1398.55</v>
       </c>
       <c r="AY6" s="17">
-        <v>1079.33962</v>
+        <v>1110.6904500000001</v>
       </c>
       <c r="AZ6" s="16">
         <v>272.83999999999997</v>
@@ -4009,7 +4245,7 @@
         <v>86.287999999999997</v>
       </c>
       <c r="BC6" s="24">
-        <v>150.2662</v>
+        <v>184.30680000000001</v>
       </c>
       <c r="BD6" s="16">
         <v>387.88</v>
@@ -4021,7 +4257,7 @@
         <v>545.20000000000005</v>
       </c>
       <c r="BG6" s="16">
-        <v>657.7</v>
+        <v>692.9</v>
       </c>
       <c r="BH6" s="16">
         <v>32691.360000000001</v>
@@ -4033,7 +4269,7 @@
         <v>1004.8419</v>
       </c>
       <c r="BK6" s="16">
-        <v>1607.19666725</v>
+        <v>2604.97123225</v>
       </c>
       <c r="BL6" s="16">
         <v>50.09</v>
@@ -4044,8 +4280,8 @@
       <c r="BN6" s="16">
         <v>131.65209200000001</v>
       </c>
-      <c r="BO6" s="16" t="s">
-        <v>137</v>
+      <c r="BO6" s="16">
+        <v>130.56135699999999</v>
       </c>
       <c r="BP6" s="16">
         <v>1.08</v>
@@ -4105,7 +4341,7 @@
         <v>519.85</v>
       </c>
       <c r="CI6" s="17">
-        <v>560.47109999999998</v>
+        <v>820.92930000000001</v>
       </c>
       <c r="CJ6" s="16">
         <v>0</v>
@@ -4177,7 +4413,7 @@
         <v>8.84</v>
       </c>
       <c r="DG6" s="17">
-        <v>33.56</v>
+        <v>46.16</v>
       </c>
       <c r="DH6" s="16">
         <v>12302.64</v>
@@ -4187,7 +4423,7 @@
       </c>
     </row>
     <row r="7" spans="2:113" ht="14.45" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B7" s="104"/>
+      <c r="B7" s="158"/>
       <c r="C7" s="8" t="s">
         <v>216</v>
       </c>
@@ -4249,7 +4485,7 @@
         <v>11.2</v>
       </c>
       <c r="W7" s="16">
-        <v>57.671999999999997</v>
+        <v>68.870157000000006</v>
       </c>
       <c r="X7" s="16">
         <v>0</v>
@@ -4257,13 +4493,13 @@
       <c r="Y7" s="17" t="s">
         <v>137</v>
       </c>
-      <c r="Z7" s="17" t="s">
-        <v>137</v>
-      </c>
-      <c r="AA7" s="17" t="s">
-        <v>137</v>
-      </c>
-      <c r="AB7" s="16" t="s">
+      <c r="Z7" s="105" t="s">
+        <v>137</v>
+      </c>
+      <c r="AA7" s="140" t="s">
+        <v>137</v>
+      </c>
+      <c r="AB7" s="123" t="s">
         <v>137</v>
       </c>
       <c r="AC7" s="17" t="s">
@@ -4333,7 +4569,7 @@
         <v>1168.558</v>
       </c>
       <c r="AY7" s="17">
-        <v>917.43867699999998</v>
+        <v>944.0868825</v>
       </c>
       <c r="AZ7" s="16">
         <v>12.04</v>
@@ -4345,7 +4581,7 @@
         <v>39.706400000000002</v>
       </c>
       <c r="BC7" s="24">
-        <v>136.62430000000001</v>
+        <v>167.21279999999999</v>
       </c>
       <c r="BD7" s="16" t="s">
         <v>137</v>
@@ -4380,8 +4616,8 @@
       <c r="BN7" s="16">
         <v>90.776180999999994</v>
       </c>
-      <c r="BO7" s="16" t="s">
-        <v>137</v>
+      <c r="BO7" s="16">
+        <v>89.925944000000001</v>
       </c>
       <c r="BP7" s="16">
         <v>1.08</v>
@@ -4523,7 +4759,7 @@
       </c>
     </row>
     <row r="8" spans="2:113" ht="14.45" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B8" s="104"/>
+      <c r="B8" s="158"/>
       <c r="C8" s="8" t="s">
         <v>5</v>
       </c>
@@ -4573,7 +4809,7 @@
         <v>336</v>
       </c>
       <c r="S8" s="16" t="s">
-        <v>374</v>
+        <v>336</v>
       </c>
       <c r="T8" s="16" t="s">
         <v>232</v>
@@ -4585,7 +4821,7 @@
         <v>307</v>
       </c>
       <c r="W8" s="16" t="s">
-        <v>352</v>
+        <v>307</v>
       </c>
       <c r="X8" s="16">
         <v>0</v>
@@ -4593,13 +4829,13 @@
       <c r="Y8" s="17" t="s">
         <v>137</v>
       </c>
-      <c r="Z8" s="17" t="s">
-        <v>137</v>
-      </c>
-      <c r="AA8" s="17" t="s">
-        <v>137</v>
-      </c>
-      <c r="AB8" s="16" t="s">
+      <c r="Z8" s="105" t="s">
+        <v>137</v>
+      </c>
+      <c r="AA8" s="140" t="s">
+        <v>137</v>
+      </c>
+      <c r="AB8" s="123" t="s">
         <v>137</v>
       </c>
       <c r="AC8" s="17" t="s">
@@ -4669,7 +4905,7 @@
         <v>292</v>
       </c>
       <c r="AY8" s="17" t="s">
-        <v>333</v>
+        <v>307</v>
       </c>
       <c r="AZ8" s="16" t="s">
         <v>232</v>
@@ -4681,7 +4917,7 @@
         <v>337</v>
       </c>
       <c r="BC8" s="24" t="s">
-        <v>343</v>
+        <v>309</v>
       </c>
       <c r="BD8" s="16" t="s">
         <v>154</v>
@@ -4693,7 +4929,7 @@
         <v>290</v>
       </c>
       <c r="BG8" s="16" t="s">
-        <v>356</v>
+        <v>340</v>
       </c>
       <c r="BH8" s="16" t="s">
         <v>233</v>
@@ -4705,7 +4941,7 @@
         <v>290</v>
       </c>
       <c r="BK8" s="16" t="s">
-        <v>375</v>
+        <v>290</v>
       </c>
       <c r="BL8" s="16" t="s">
         <v>181</v>
@@ -4717,7 +4953,7 @@
         <v>335</v>
       </c>
       <c r="BO8" s="16" t="s">
-        <v>137</v>
+        <v>335</v>
       </c>
       <c r="BP8" s="16" t="s">
         <v>153</v>
@@ -4729,7 +4965,7 @@
         <v>137</v>
       </c>
       <c r="BS8" s="17" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="BT8" s="16">
         <v>0</v>
@@ -4777,7 +5013,7 @@
         <v>292</v>
       </c>
       <c r="CI8" s="17" t="s">
-        <v>368</v>
+        <v>292</v>
       </c>
       <c r="CJ8" s="16" t="s">
         <v>234</v>
@@ -4813,7 +5049,7 @@
         <v>307</v>
       </c>
       <c r="CU8" s="16" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="CV8" s="16" t="s">
         <v>235</v>
@@ -4837,7 +5073,7 @@
         <v>290</v>
       </c>
       <c r="DC8" s="16" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="DD8" s="16" t="s">
         <v>137</v>
@@ -4849,7 +5085,7 @@
         <v>312</v>
       </c>
       <c r="DG8" s="17" t="s">
-        <v>368</v>
+        <v>292</v>
       </c>
       <c r="DH8" s="16" t="s">
         <v>181</v>
@@ -4859,7 +5095,7 @@
       </c>
     </row>
     <row r="9" spans="2:113" ht="22.85" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B9" s="109" t="s">
+      <c r="B9" s="163" t="s">
         <v>6</v>
       </c>
       <c r="C9" s="8" t="s">
@@ -4931,13 +5167,13 @@
       <c r="Y9" s="17" t="s">
         <v>137</v>
       </c>
-      <c r="Z9" s="17">
+      <c r="Z9" s="105">
         <v>245.1</v>
       </c>
-      <c r="AA9" s="17" t="s">
-        <v>137</v>
-      </c>
-      <c r="AB9" s="16" t="s">
+      <c r="AA9" s="140">
+        <v>4.72</v>
+      </c>
+      <c r="AB9" s="123" t="s">
         <v>137</v>
       </c>
       <c r="AC9" s="17" t="s">
@@ -4971,7 +5207,7 @@
         <v>12.4</v>
       </c>
       <c r="AM9" s="17">
-        <v>1.1000000000000001</v>
+        <v>2.15</v>
       </c>
       <c r="AN9" s="16">
         <v>228</v>
@@ -4983,7 +5219,7 @@
         <v>758.95111699999995</v>
       </c>
       <c r="AQ9" s="16">
-        <v>1059.6138182</v>
+        <v>1154.7580602</v>
       </c>
       <c r="AR9" s="16" t="s">
         <v>137</v>
@@ -5007,7 +5243,7 @@
         <v>696.01</v>
       </c>
       <c r="AY9" s="17">
-        <v>423.80489999999998</v>
+        <v>462.49009999999998</v>
       </c>
       <c r="AZ9" s="16">
         <v>145.44</v>
@@ -5031,7 +5267,7 @@
         <v>732.7</v>
       </c>
       <c r="BG9" s="94">
-        <v>800.8</v>
+        <v>811.3</v>
       </c>
       <c r="BH9" s="16">
         <v>151350.82</v>
@@ -5043,7 +5279,7 @@
         <v>3326.6045600000002</v>
       </c>
       <c r="BK9" s="16">
-        <v>2834.4006395400002</v>
+        <v>3392.4550969299999</v>
       </c>
       <c r="BL9" s="16">
         <v>0.74</v>
@@ -5054,8 +5290,8 @@
       <c r="BN9" s="17" t="s">
         <v>137</v>
       </c>
-      <c r="BO9" s="17" t="s">
-        <v>137</v>
+      <c r="BO9" s="17">
+        <v>3.2</v>
       </c>
       <c r="BP9" s="16">
         <v>3.12</v>
@@ -5115,7 +5351,7 @@
         <v>221.42</v>
       </c>
       <c r="CI9" s="17">
-        <v>623.06719999999996</v>
+        <v>702.39160000000004</v>
       </c>
       <c r="CJ9" s="16">
         <v>111.33</v>
@@ -5127,7 +5363,7 @@
         <v>124.947</v>
       </c>
       <c r="CM9" s="17">
-        <v>126.199</v>
+        <v>130.30500000000001</v>
       </c>
       <c r="CN9" s="16">
         <v>1917.43</v>
@@ -5175,7 +5411,7 @@
         <v>2494.4960000000001</v>
       </c>
       <c r="DC9" s="16">
-        <v>2483.9290000000001</v>
+        <v>2529.7570000000001</v>
       </c>
       <c r="DD9" s="16">
         <v>101</v>
@@ -5197,7 +5433,7 @@
       </c>
     </row>
     <row r="10" spans="2:113" ht="13.85" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B10" s="110"/>
+      <c r="B10" s="164"/>
       <c r="C10" s="8" t="s">
         <v>216</v>
       </c>
@@ -5267,13 +5503,13 @@
       <c r="Y10" s="17" t="s">
         <v>137</v>
       </c>
-      <c r="Z10" s="17">
-        <v>0</v>
-      </c>
-      <c r="AA10" s="17" t="s">
-        <v>137</v>
-      </c>
-      <c r="AB10" s="16" t="s">
+      <c r="Z10" s="105">
+        <v>0</v>
+      </c>
+      <c r="AA10" s="140" t="s">
+        <v>137</v>
+      </c>
+      <c r="AB10" s="123" t="s">
         <v>137</v>
       </c>
       <c r="AC10" s="17" t="s">
@@ -5343,7 +5579,7 @@
         <v>563.52949999999998</v>
       </c>
       <c r="AY10" s="17">
-        <v>346.12433499999997</v>
+        <v>375.37130500000001</v>
       </c>
       <c r="AZ10" s="16">
         <v>30.07</v>
@@ -5379,7 +5615,7 @@
         <v>144.7867</v>
       </c>
       <c r="BK10" s="16">
-        <v>210.56724156000001</v>
+        <v>214.3526937</v>
       </c>
       <c r="BL10" s="16" t="s">
         <v>137</v>
@@ -5463,7 +5699,7 @@
         <v>39.066000000000003</v>
       </c>
       <c r="CM10" s="17">
-        <v>41.595999999999997</v>
+        <v>44.720999999999997</v>
       </c>
       <c r="CN10" s="16">
         <v>898.38999999999896</v>
@@ -5511,7 +5747,7 @@
         <v>52.3</v>
       </c>
       <c r="DC10" s="16">
-        <v>319.7</v>
+        <v>322.10000000000002</v>
       </c>
       <c r="DD10" s="16" t="s">
         <v>137</v>
@@ -5533,7 +5769,7 @@
       </c>
     </row>
     <row r="11" spans="2:113" ht="14.45" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B11" s="111"/>
+      <c r="B11" s="165"/>
       <c r="C11" s="8" t="s">
         <v>5</v>
       </c>
@@ -5559,7 +5795,7 @@
         <v>341</v>
       </c>
       <c r="K11" s="17" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="L11" s="16" t="s">
         <v>239</v>
@@ -5571,7 +5807,7 @@
         <v>290</v>
       </c>
       <c r="O11" s="16" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="P11" s="16" t="s">
         <v>196</v>
@@ -5583,7 +5819,7 @@
         <v>330</v>
       </c>
       <c r="S11" s="17" t="s">
-        <v>361</v>
+        <v>330</v>
       </c>
       <c r="T11" s="16" t="s">
         <v>231</v>
@@ -5595,7 +5831,7 @@
         <v>307</v>
       </c>
       <c r="W11" s="16" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="X11" s="16">
         <v>0</v>
@@ -5603,13 +5839,13 @@
       <c r="Y11" s="17" t="s">
         <v>137</v>
       </c>
-      <c r="Z11" s="17" t="s">
+      <c r="Z11" s="105" t="s">
         <v>342</v>
       </c>
-      <c r="AA11" s="17" t="s">
-        <v>137</v>
-      </c>
-      <c r="AB11" s="16" t="s">
+      <c r="AA11" s="140" t="s">
+        <v>335</v>
+      </c>
+      <c r="AB11" s="123" t="s">
         <v>137</v>
       </c>
       <c r="AC11" s="17" t="s">
@@ -5631,7 +5867,7 @@
         <v>0</v>
       </c>
       <c r="AI11" s="17" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="AJ11" s="16" t="s">
         <v>191</v>
@@ -5643,7 +5879,7 @@
         <v>312</v>
       </c>
       <c r="AM11" s="17" t="s">
-        <v>331</v>
+        <v>312</v>
       </c>
       <c r="AN11" s="16" t="s">
         <v>240</v>
@@ -5655,7 +5891,7 @@
         <v>332</v>
       </c>
       <c r="AQ11" s="16" t="s">
-        <v>377</v>
+        <v>381</v>
       </c>
       <c r="AR11" s="16" t="s">
         <v>137</v>
@@ -5679,7 +5915,7 @@
         <v>292</v>
       </c>
       <c r="AY11" s="17" t="s">
-        <v>375</v>
+        <v>290</v>
       </c>
       <c r="AZ11" s="16" t="s">
         <v>231</v>
@@ -5691,7 +5927,7 @@
         <v>309</v>
       </c>
       <c r="BC11" s="24" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="BD11" s="16" t="s">
         <v>231</v>
@@ -5703,7 +5939,7 @@
         <v>333</v>
       </c>
       <c r="BG11" s="16" t="s">
-        <v>378</v>
+        <v>382</v>
       </c>
       <c r="BH11" s="16" t="s">
         <v>193</v>
@@ -5715,7 +5951,7 @@
         <v>332</v>
       </c>
       <c r="BK11" s="16" t="s">
-        <v>378</v>
+        <v>382</v>
       </c>
       <c r="BL11" s="16" t="s">
         <v>172</v>
@@ -5727,7 +5963,7 @@
         <v>137</v>
       </c>
       <c r="BO11" s="17" t="s">
-        <v>137</v>
+        <v>335</v>
       </c>
       <c r="BP11" s="16" t="s">
         <v>193</v>
@@ -5787,7 +6023,7 @@
         <v>287</v>
       </c>
       <c r="CI11" s="17" t="s">
-        <v>376</v>
+        <v>332</v>
       </c>
       <c r="CJ11" s="16" t="s">
         <v>188</v>
@@ -5799,7 +6035,7 @@
         <v>292</v>
       </c>
       <c r="CM11" s="17" t="s">
-        <v>376</v>
+        <v>332</v>
       </c>
       <c r="CN11" s="16" t="s">
         <v>194</v>
@@ -5823,7 +6059,7 @@
         <v>290</v>
       </c>
       <c r="CU11" s="16" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="CV11" s="16" t="s">
         <v>193</v>
@@ -5847,7 +6083,7 @@
         <v>287</v>
       </c>
       <c r="DC11" s="16" t="s">
-        <v>376</v>
+        <v>332</v>
       </c>
       <c r="DD11" s="16" t="s">
         <v>192</v>
@@ -5869,10 +6105,10 @@
       </c>
     </row>
     <row r="12" spans="2:113" ht="14.45" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B12" s="107" t="s">
+      <c r="B12" s="161" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="108"/>
+      <c r="C12" s="162"/>
       <c r="D12" s="21">
         <f t="shared" ref="D12:BO12" si="0">IF(D6="n/a",0,IF(D6="no data",0,D6))+IF(D9="n/a",0,IF(D9="no data",0,D9))</f>
         <v>0</v>
@@ -5951,7 +6187,7 @@
       </c>
       <c r="W12" s="16">
         <f t="shared" si="0"/>
-        <v>612.87215200000003</v>
+        <v>631.08008599999994</v>
       </c>
       <c r="X12" s="16">
         <f t="shared" si="0"/>
@@ -5961,15 +6197,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="Z12" s="16">
+      <c r="Z12" s="106">
         <f t="shared" si="0"/>
         <v>245.1</v>
       </c>
-      <c r="AA12" s="16">
+      <c r="AA12" s="141">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AB12" s="16">
+        <v>4.72</v>
+      </c>
+      <c r="AB12" s="123">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -6015,7 +6251,7 @@
       </c>
       <c r="AM12" s="16">
         <f t="shared" si="0"/>
-        <v>1.1000000000000001</v>
+        <v>2.15</v>
       </c>
       <c r="AN12" s="16">
         <f t="shared" si="0"/>
@@ -6031,7 +6267,7 @@
       </c>
       <c r="AQ12" s="16">
         <f t="shared" si="0"/>
-        <v>1099.2784062000001</v>
+        <v>1194.4226482000001</v>
       </c>
       <c r="AR12" s="16">
         <f t="shared" si="0"/>
@@ -6063,7 +6299,7 @@
       </c>
       <c r="AY12" s="16">
         <f t="shared" si="0"/>
-        <v>1503.1445199999998</v>
+        <v>1573.18055</v>
       </c>
       <c r="AZ12" s="16">
         <f t="shared" si="0"/>
@@ -6079,7 +6315,7 @@
       </c>
       <c r="BC12" s="16">
         <f t="shared" si="0"/>
-        <v>339.30451700000003</v>
+        <v>373.34511700000002</v>
       </c>
       <c r="BD12" s="16">
         <f t="shared" si="0"/>
@@ -6095,7 +6331,7 @@
       </c>
       <c r="BG12" s="16">
         <f t="shared" si="0"/>
-        <v>1458.5</v>
+        <v>1504.1999999999998</v>
       </c>
       <c r="BH12" s="16">
         <f t="shared" si="0"/>
@@ -6111,7 +6347,7 @@
       </c>
       <c r="BK12" s="16">
         <f t="shared" si="0"/>
-        <v>4441.5973067900004</v>
+        <v>5997.4263291799998</v>
       </c>
       <c r="BL12" s="16">
         <f t="shared" si="0"/>
@@ -6127,7 +6363,7 @@
       </c>
       <c r="BO12" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>133.76135699999998</v>
       </c>
       <c r="BP12" s="16">
         <f t="shared" ref="BP12:DI12" si="1">IF(BP6="n/a",0,IF(BP6="no data",0,BP6))+IF(BP9="n/a",0,IF(BP9="no data",0,BP9))</f>
@@ -6203,7 +6439,7 @@
       </c>
       <c r="CI12" s="16">
         <f t="shared" si="1"/>
-        <v>1183.5382999999999</v>
+        <v>1523.3209000000002</v>
       </c>
       <c r="CJ12" s="16">
         <f t="shared" si="1"/>
@@ -6219,7 +6455,7 @@
       </c>
       <c r="CM12" s="16">
         <f t="shared" si="1"/>
-        <v>126.199</v>
+        <v>130.30500000000001</v>
       </c>
       <c r="CN12" s="16">
         <f t="shared" si="1"/>
@@ -6283,7 +6519,7 @@
       </c>
       <c r="DC12" s="16">
         <f t="shared" si="1"/>
-        <v>2732.527</v>
+        <v>2778.355</v>
       </c>
       <c r="DD12" s="16">
         <f t="shared" si="1"/>
@@ -6299,7 +6535,7 @@
       </c>
       <c r="DG12" s="16">
         <f t="shared" si="1"/>
-        <v>79.72</v>
+        <v>92.32</v>
       </c>
       <c r="DH12" s="16">
         <f t="shared" si="1"/>
@@ -6311,10 +6547,10 @@
       </c>
     </row>
     <row r="13" spans="2:113" ht="14.45" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B13" s="107" t="s">
+      <c r="B13" s="161" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="108"/>
+      <c r="C13" s="162"/>
       <c r="D13" s="9" t="s">
         <v>137</v>
       </c>
@@ -6337,7 +6573,7 @@
         <v>341</v>
       </c>
       <c r="K13" s="17" t="s">
-        <v>388</v>
+        <v>379</v>
       </c>
       <c r="L13" s="9" t="s">
         <v>140</v>
@@ -6349,7 +6585,7 @@
         <v>290</v>
       </c>
       <c r="O13" s="9" t="s">
-        <v>379</v>
+        <v>374</v>
       </c>
       <c r="P13" s="9" t="s">
         <v>141</v>
@@ -6361,7 +6597,7 @@
         <v>330</v>
       </c>
       <c r="S13" s="9" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="T13" s="32" t="s">
         <v>196</v>
@@ -6373,7 +6609,7 @@
         <v>307</v>
       </c>
       <c r="W13" s="9" t="s">
-        <v>380</v>
+        <v>265</v>
       </c>
       <c r="X13" s="17" t="s">
         <v>137</v>
@@ -6381,13 +6617,13 @@
       <c r="Y13" s="17" t="s">
         <v>137</v>
       </c>
-      <c r="Z13" s="17" t="s">
+      <c r="Z13" s="105" t="s">
         <v>342</v>
       </c>
-      <c r="AA13" s="17" t="s">
-        <v>137</v>
-      </c>
-      <c r="AB13" s="17" t="s">
+      <c r="AA13" s="140" t="s">
+        <v>153</v>
+      </c>
+      <c r="AB13" s="124" t="s">
         <v>137</v>
       </c>
       <c r="AC13" s="17" t="s">
@@ -6409,7 +6645,7 @@
         <v>0</v>
       </c>
       <c r="AI13" s="17" t="s">
-        <v>381</v>
+        <v>375</v>
       </c>
       <c r="AJ13" s="9" t="s">
         <v>191</v>
@@ -6421,7 +6657,7 @@
         <v>312</v>
       </c>
       <c r="AM13" s="17" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="AN13" s="16" t="s">
         <v>240</v>
@@ -6433,7 +6669,7 @@
         <v>332</v>
       </c>
       <c r="AQ13" s="16" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="AR13" s="17" t="s">
         <v>137</v>
@@ -6457,7 +6693,7 @@
         <v>292</v>
       </c>
       <c r="AY13" s="17" t="s">
-        <v>380</v>
+        <v>265</v>
       </c>
       <c r="AZ13" s="9" t="s">
         <v>195</v>
@@ -6469,7 +6705,7 @@
         <v>309</v>
       </c>
       <c r="BC13" s="26" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="BD13" s="9" t="s">
         <v>177</v>
@@ -6481,7 +6717,7 @@
         <v>290</v>
       </c>
       <c r="BG13" s="9" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="BH13" s="9" t="s">
         <v>183</v>
@@ -6493,7 +6729,7 @@
         <v>332</v>
       </c>
       <c r="BK13" s="9" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="BL13" s="9" t="s">
         <v>181</v>
@@ -6505,7 +6741,7 @@
         <v>335</v>
       </c>
       <c r="BO13" s="9" t="s">
-        <v>137</v>
+        <v>153</v>
       </c>
       <c r="BP13" s="9" t="s">
         <v>193</v>
@@ -6517,7 +6753,7 @@
         <v>137</v>
       </c>
       <c r="BS13" s="17" t="s">
-        <v>384</v>
+        <v>376</v>
       </c>
       <c r="BT13" s="17" t="s">
         <v>137</v>
@@ -6541,7 +6777,7 @@
         <v>334</v>
       </c>
       <c r="CA13" s="17" t="s">
-        <v>385</v>
+        <v>377</v>
       </c>
       <c r="CB13" s="34" t="s">
         <v>139</v>
@@ -6565,7 +6801,7 @@
         <v>287</v>
       </c>
       <c r="CI13" s="17" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="CJ13" s="17" t="s">
         <v>188</v>
@@ -6577,7 +6813,7 @@
         <v>292</v>
       </c>
       <c r="CM13" s="17" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="CN13" s="9" t="s">
         <v>194</v>
@@ -6601,7 +6837,7 @@
         <v>290</v>
       </c>
       <c r="CU13" s="9" t="s">
-        <v>387</v>
+        <v>378</v>
       </c>
       <c r="CV13" s="9" t="s">
         <v>193</v>
@@ -6625,7 +6861,7 @@
         <v>290</v>
       </c>
       <c r="DC13" s="9" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="DD13" s="9" t="s">
         <v>192</v>
@@ -6637,7 +6873,7 @@
         <v>309</v>
       </c>
       <c r="DG13" s="16" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="DH13" s="9" t="s">
         <v>192</v>
@@ -6673,9 +6909,9 @@
       <c r="W14" s="7"/>
       <c r="X14" s="7"/>
       <c r="Y14" s="7"/>
-      <c r="Z14" s="7"/>
-      <c r="AA14" s="7"/>
-      <c r="AB14" s="7"/>
+      <c r="Z14" s="104"/>
+      <c r="AA14" s="139"/>
+      <c r="AB14" s="122"/>
       <c r="AC14" s="7"/>
       <c r="AD14" s="7"/>
       <c r="AE14" s="7"/>
@@ -6763,7 +6999,7 @@
       <c r="DI14" s="7"/>
     </row>
     <row r="15" spans="2:113" ht="22.85" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B15" s="104" t="s">
+      <c r="B15" s="158" t="s">
         <v>3</v>
       </c>
       <c r="C15" s="8" t="s">
@@ -6835,13 +7071,13 @@
       <c r="Y15" s="17">
         <v>0</v>
       </c>
-      <c r="Z15" s="17">
-        <v>0</v>
-      </c>
-      <c r="AA15" s="17">
-        <v>0</v>
-      </c>
-      <c r="AB15" s="17" t="s">
+      <c r="Z15" s="105">
+        <v>0</v>
+      </c>
+      <c r="AA15" s="140">
+        <v>0</v>
+      </c>
+      <c r="AB15" s="124" t="s">
         <v>137</v>
       </c>
       <c r="AC15" s="17">
@@ -7101,7 +7337,7 @@
       </c>
     </row>
     <row r="16" spans="2:113" ht="22.85" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B16" s="104"/>
+      <c r="B16" s="158"/>
       <c r="C16" s="8" t="s">
         <v>12</v>
       </c>
@@ -7171,13 +7407,13 @@
       <c r="Y16" s="17">
         <v>0</v>
       </c>
-      <c r="Z16" s="17">
-        <v>0</v>
-      </c>
-      <c r="AA16" s="17">
-        <v>0</v>
-      </c>
-      <c r="AB16" s="17" t="s">
+      <c r="Z16" s="105">
+        <v>0</v>
+      </c>
+      <c r="AA16" s="140">
+        <v>0</v>
+      </c>
+      <c r="AB16" s="124" t="s">
         <v>137</v>
       </c>
       <c r="AC16" s="17">
@@ -7437,7 +7673,7 @@
       </c>
     </row>
     <row r="17" spans="2:113" ht="22.85" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B17" s="104" t="s">
+      <c r="B17" s="158" t="s">
         <v>6</v>
       </c>
       <c r="C17" s="8" t="s">
@@ -7509,13 +7745,13 @@
       <c r="Y17" s="17">
         <v>0</v>
       </c>
-      <c r="Z17" s="17">
+      <c r="Z17" s="105">
         <v>1</v>
       </c>
-      <c r="AA17" s="17">
+      <c r="AA17" s="140">
         <v>1</v>
       </c>
-      <c r="AB17" s="17" t="s">
+      <c r="AB17" s="124" t="s">
         <v>137</v>
       </c>
       <c r="AC17" s="17">
@@ -7775,7 +8011,7 @@
       </c>
     </row>
     <row r="18" spans="2:113" ht="22.85" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B18" s="104"/>
+      <c r="B18" s="158"/>
       <c r="C18" s="8" t="s">
         <v>14</v>
       </c>
@@ -7845,13 +8081,13 @@
       <c r="Y18" s="17">
         <v>0</v>
       </c>
-      <c r="Z18" s="17">
-        <v>0</v>
-      </c>
-      <c r="AA18" s="17">
-        <v>0</v>
-      </c>
-      <c r="AB18" s="17" t="s">
+      <c r="Z18" s="105">
+        <v>0</v>
+      </c>
+      <c r="AA18" s="140">
+        <v>0</v>
+      </c>
+      <c r="AB18" s="124" t="s">
         <v>137</v>
       </c>
       <c r="AC18" s="17">
@@ -8137,9 +8373,9 @@
       <c r="W19" s="7"/>
       <c r="X19" s="7"/>
       <c r="Y19" s="7"/>
-      <c r="Z19" s="7"/>
-      <c r="AA19" s="7"/>
-      <c r="AB19" s="7"/>
+      <c r="Z19" s="104"/>
+      <c r="AA19" s="139"/>
+      <c r="AB19" s="122"/>
       <c r="AC19" s="7"/>
       <c r="AD19" s="7"/>
       <c r="AE19" s="7"/>
@@ -8227,7 +8463,7 @@
       <c r="DI19" s="7"/>
     </row>
     <row r="20" spans="2:113" ht="22" x14ac:dyDescent="0.5">
-      <c r="B20" s="104" t="s">
+      <c r="B20" s="158" t="s">
         <v>3</v>
       </c>
       <c r="C20" s="8" t="s">
@@ -8301,14 +8537,14 @@
       <c r="Y20" s="17">
         <v>0</v>
       </c>
-      <c r="Z20" s="17">
+      <c r="Z20" s="105">
         <f>'Feuil3-2020'!L8</f>
         <v>0</v>
       </c>
-      <c r="AA20" s="17" t="s">
-        <v>137</v>
-      </c>
-      <c r="AB20" s="17">
+      <c r="AA20" s="140" t="s">
+        <v>137</v>
+      </c>
+      <c r="AB20" s="124">
         <v>0</v>
       </c>
       <c r="AC20" s="17">
@@ -8589,7 +8825,7 @@
       </c>
     </row>
     <row r="21" spans="2:113" ht="22" x14ac:dyDescent="0.5">
-      <c r="B21" s="104"/>
+      <c r="B21" s="158"/>
       <c r="C21" s="8" t="s">
         <v>17</v>
       </c>
@@ -8675,14 +8911,14 @@
         <f>'Feuil3-2020'!E8</f>
         <v>0</v>
       </c>
-      <c r="Z21" s="17">
+      <c r="Z21" s="105">
         <f>'Feuil3-2020'!F8</f>
         <v>0</v>
       </c>
-      <c r="AA21" s="17" t="s">
-        <v>137</v>
-      </c>
-      <c r="AB21" s="17">
+      <c r="AA21" s="140" t="s">
+        <v>137</v>
+      </c>
+      <c r="AB21" s="124">
         <f>'Feuil3-2020'!D9</f>
         <v>0</v>
       </c>
@@ -9007,7 +9243,7 @@
       </c>
     </row>
     <row r="22" spans="2:113" ht="22" x14ac:dyDescent="0.5">
-      <c r="B22" s="105" t="s">
+      <c r="B22" s="159" t="s">
         <v>6</v>
       </c>
       <c r="C22" s="8" t="s">
@@ -9079,13 +9315,13 @@
       <c r="Y22" s="17" t="s">
         <v>137</v>
       </c>
-      <c r="Z22" s="17">
+      <c r="Z22" s="105">
         <v>1641600</v>
       </c>
-      <c r="AA22" s="17">
+      <c r="AA22" s="140">
         <v>10000</v>
       </c>
-      <c r="AB22" s="17" t="s">
+      <c r="AB22" s="124" t="s">
         <v>137</v>
       </c>
       <c r="AC22" s="17" t="s">
@@ -9345,7 +9581,7 @@
       </c>
     </row>
     <row r="23" spans="2:113" x14ac:dyDescent="0.5">
-      <c r="B23" s="105"/>
+      <c r="B23" s="159"/>
       <c r="C23" s="8" t="s">
         <v>19</v>
       </c>
@@ -9415,13 +9651,13 @@
       <c r="Y23" s="17" t="s">
         <v>137</v>
       </c>
-      <c r="Z23" s="17">
+      <c r="Z23" s="105">
         <v>1750000</v>
       </c>
-      <c r="AA23" s="17">
+      <c r="AA23" s="140">
         <v>35000</v>
       </c>
-      <c r="AB23" s="17" t="s">
+      <c r="AB23" s="124" t="s">
         <v>137</v>
       </c>
       <c r="AC23" s="17" t="s">
@@ -9682,10 +9918,10 @@
     </row>
     <row r="24" spans="2:113" ht="14.45" customHeight="1" x14ac:dyDescent="0.5"/>
     <row r="25" spans="2:113" ht="14.45" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B25" s="112" t="s">
-        <v>0</v>
-      </c>
-      <c r="C25" s="112"/>
+      <c r="B25" s="166" t="s">
+        <v>0</v>
+      </c>
+      <c r="C25" s="166"/>
       <c r="D25" s="5">
         <f>D$3</f>
         <v>2016</v>
@@ -9774,15 +10010,15 @@
         <f t="shared" si="2"/>
         <v>2018</v>
       </c>
-      <c r="Z25" s="5">
+      <c r="Z25" s="107">
         <f t="shared" si="2"/>
         <v>2020</v>
       </c>
-      <c r="AA25" s="5">
+      <c r="AA25" s="143">
         <f t="shared" si="2"/>
         <v>2022</v>
       </c>
-      <c r="AB25" s="5">
+      <c r="AB25" s="125">
         <f t="shared" si="2"/>
         <v>2016</v>
       </c>
@@ -10128,10 +10364,10 @@
       </c>
     </row>
     <row r="26" spans="2:113" ht="25" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B26" s="116" t="s">
+      <c r="B26" s="170" t="s">
         <v>20</v>
       </c>
-      <c r="C26" s="116"/>
+      <c r="C26" s="170"/>
       <c r="D26" s="11"/>
       <c r="E26" s="11"/>
       <c r="F26" s="11"/>
@@ -10154,9 +10390,9 @@
       <c r="W26" s="11"/>
       <c r="X26" s="11"/>
       <c r="Y26" s="11"/>
-      <c r="Z26" s="11"/>
-      <c r="AA26" s="11"/>
-      <c r="AB26" s="11"/>
+      <c r="Z26" s="108"/>
+      <c r="AA26" s="144"/>
+      <c r="AB26" s="126"/>
       <c r="AC26" s="11"/>
       <c r="AD26" s="11"/>
       <c r="AE26" s="11"/>
@@ -10244,7 +10480,7 @@
       <c r="DI26" s="11"/>
     </row>
     <row r="27" spans="2:113" ht="22" x14ac:dyDescent="0.5">
-      <c r="B27" s="113" t="s">
+      <c r="B27" s="167" t="s">
         <v>3</v>
       </c>
       <c r="C27" s="12" t="s">
@@ -10316,13 +10552,13 @@
       <c r="Y27" s="18" t="s">
         <v>205</v>
       </c>
-      <c r="Z27" s="28" t="s">
-        <v>137</v>
-      </c>
-      <c r="AA27" s="28">
+      <c r="Z27" s="109" t="s">
+        <v>137</v>
+      </c>
+      <c r="AA27" s="145">
         <v>325</v>
       </c>
-      <c r="AB27" s="18">
+      <c r="AB27" s="127">
         <v>413.33333333333331</v>
       </c>
       <c r="AC27" s="18">
@@ -10582,7 +10818,7 @@
       </c>
     </row>
     <row r="28" spans="2:113" x14ac:dyDescent="0.5">
-      <c r="B28" s="113"/>
+      <c r="B28" s="167"/>
       <c r="C28" s="12" t="s">
         <v>22</v>
       </c>
@@ -10606,7 +10842,7 @@
         <v>291</v>
       </c>
       <c r="K28" s="18" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="L28" s="18" t="s">
         <v>137</v>
@@ -10642,7 +10878,7 @@
         <v>300</v>
       </c>
       <c r="W28" s="18" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="X28" s="18" t="s">
         <v>247</v>
@@ -10650,13 +10886,13 @@
       <c r="Y28" s="18" t="s">
         <v>190</v>
       </c>
-      <c r="Z28" s="28" t="s">
-        <v>137</v>
-      </c>
-      <c r="AA28" s="28" t="s">
-        <v>365</v>
-      </c>
-      <c r="AB28" s="18" t="s">
+      <c r="Z28" s="109" t="s">
+        <v>137</v>
+      </c>
+      <c r="AA28" s="145" t="s">
+        <v>363</v>
+      </c>
+      <c r="AB28" s="127" t="s">
         <v>248</v>
       </c>
       <c r="AC28" s="18" t="s">
@@ -10690,7 +10926,7 @@
         <v>297</v>
       </c>
       <c r="AM28" s="18" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="AN28" s="18" t="s">
         <v>137</v>
@@ -10762,7 +10998,7 @@
         <v>296</v>
       </c>
       <c r="BK28" s="18" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="BL28" s="18" t="s">
         <v>252</v>
@@ -10786,7 +11022,7 @@
         <v>285</v>
       </c>
       <c r="BS28" s="18" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="BT28" s="18" t="s">
         <v>165</v>
@@ -10810,7 +11046,7 @@
         <v>295</v>
       </c>
       <c r="CA28" s="18" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="CB28" s="18" t="s">
         <v>253</v>
@@ -10822,7 +11058,7 @@
         <v>273</v>
       </c>
       <c r="CE28" s="18" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="CF28" s="18" t="s">
         <v>137</v>
@@ -10846,7 +11082,7 @@
         <v>137</v>
       </c>
       <c r="CM28" s="28" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="CN28" s="18" t="s">
         <v>246</v>
@@ -10916,7 +11152,7 @@
       </c>
     </row>
     <row r="29" spans="2:113" ht="22" x14ac:dyDescent="0.5">
-      <c r="B29" s="113"/>
+      <c r="B29" s="167"/>
       <c r="C29" s="12" t="s">
         <v>23</v>
       </c>
@@ -10984,13 +11220,13 @@
       <c r="Y29" s="18" t="s">
         <v>206</v>
       </c>
-      <c r="Z29" s="18">
+      <c r="Z29" s="110">
         <v>300</v>
       </c>
-      <c r="AA29" s="18">
+      <c r="AA29" s="146">
         <v>325</v>
       </c>
-      <c r="AB29" s="18">
+      <c r="AB29" s="127">
         <v>540.5</v>
       </c>
       <c r="AC29" s="18">
@@ -11036,7 +11272,7 @@
         <v>316</v>
       </c>
       <c r="AQ29" s="18" t="s">
-        <v>394</v>
+        <v>380</v>
       </c>
       <c r="AR29" s="28">
         <v>1989</v>
@@ -11250,7 +11486,7 @@
       </c>
     </row>
     <row r="30" spans="2:113" x14ac:dyDescent="0.5">
-      <c r="B30" s="113"/>
+      <c r="B30" s="167"/>
       <c r="C30" s="12" t="s">
         <v>24</v>
       </c>
@@ -11310,7 +11546,7 @@
         <v>305</v>
       </c>
       <c r="W30" s="28" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="X30" s="18" t="s">
         <v>199</v>
@@ -11318,13 +11554,13 @@
       <c r="Y30" s="18" t="s">
         <v>199</v>
       </c>
-      <c r="Z30" s="18" t="s">
+      <c r="Z30" s="110" t="s">
         <v>302</v>
       </c>
-      <c r="AA30" s="18" t="s">
+      <c r="AA30" s="146" t="s">
         <v>286</v>
       </c>
-      <c r="AB30" s="18" t="s">
+      <c r="AB30" s="127" t="s">
         <v>165</v>
       </c>
       <c r="AC30" s="18" t="s">
@@ -11334,7 +11570,7 @@
         <v>303</v>
       </c>
       <c r="AE30" s="18" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="AF30" s="18" t="s">
         <v>199</v>
@@ -11406,7 +11642,7 @@
         <v>304</v>
       </c>
       <c r="BC30" s="28" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="BD30" s="18" t="s">
         <v>137</v>
@@ -11418,7 +11654,7 @@
         <v>305</v>
       </c>
       <c r="BG30" s="28" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="BH30" s="18" t="s">
         <v>259</v>
@@ -11478,7 +11714,7 @@
         <v>135</v>
       </c>
       <c r="CA30" s="18" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="CB30" s="18" t="s">
         <v>260</v>
@@ -11514,7 +11750,7 @@
         <v>137</v>
       </c>
       <c r="CM30" s="28" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="CN30" s="18" t="s">
         <v>259</v>
@@ -11574,7 +11810,7 @@
         <v>302</v>
       </c>
       <c r="DG30" s="18" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="DH30" s="18" t="s">
         <v>259</v>
@@ -11584,7 +11820,7 @@
       </c>
     </row>
     <row r="31" spans="2:113" ht="22" x14ac:dyDescent="0.5">
-      <c r="B31" s="113"/>
+      <c r="B31" s="167"/>
       <c r="C31" s="12" t="s">
         <v>25</v>
       </c>
@@ -11652,13 +11888,13 @@
       <c r="Y31" s="18" t="s">
         <v>207</v>
       </c>
-      <c r="Z31" s="18">
+      <c r="Z31" s="110">
         <v>284.28570999999999</v>
       </c>
-      <c r="AA31" s="18">
+      <c r="AA31" s="146">
         <v>325</v>
       </c>
-      <c r="AB31" s="18">
+      <c r="AB31" s="127">
         <v>510</v>
       </c>
       <c r="AC31" s="18">
@@ -11918,7 +12154,7 @@
       </c>
     </row>
     <row r="32" spans="2:113" x14ac:dyDescent="0.5">
-      <c r="B32" s="113"/>
+      <c r="B32" s="167"/>
       <c r="C32" s="12" t="s">
         <v>22</v>
       </c>
@@ -11942,7 +12178,7 @@
         <v>292</v>
       </c>
       <c r="K32" s="18" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="L32" s="18" t="s">
         <v>265</v>
@@ -11954,7 +12190,7 @@
         <v>307</v>
       </c>
       <c r="O32" s="18" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="P32" s="18" t="s">
         <v>266</v>
@@ -11966,7 +12202,7 @@
         <v>345</v>
       </c>
       <c r="S32" s="18" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="T32" s="18" t="s">
         <v>195</v>
@@ -11978,7 +12214,7 @@
         <v>307</v>
       </c>
       <c r="W32" s="18" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="X32" s="18" t="s">
         <v>200</v>
@@ -11986,13 +12222,13 @@
       <c r="Y32" s="18" t="s">
         <v>200</v>
       </c>
-      <c r="Z32" s="18" t="s">
+      <c r="Z32" s="110" t="s">
         <v>284</v>
       </c>
-      <c r="AA32" s="18" t="s">
-        <v>358</v>
-      </c>
-      <c r="AB32" s="18" t="s">
+      <c r="AA32" s="146" t="s">
+        <v>357</v>
+      </c>
+      <c r="AB32" s="127" t="s">
         <v>160</v>
       </c>
       <c r="AC32" s="18" t="s">
@@ -12026,7 +12262,7 @@
         <v>309</v>
       </c>
       <c r="AM32" s="18" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="AN32" s="18" t="s">
         <v>213</v>
@@ -12086,7 +12322,7 @@
         <v>292</v>
       </c>
       <c r="BG32" s="18" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="BH32" s="18" t="s">
         <v>267</v>
@@ -12098,7 +12334,7 @@
         <v>292</v>
       </c>
       <c r="BK32" s="18" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="BL32" s="18" t="s">
         <v>182</v>
@@ -12158,7 +12394,7 @@
         <v>312</v>
       </c>
       <c r="CE32" s="18" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="CF32" s="18" t="s">
         <v>271</v>
@@ -12182,7 +12418,7 @@
         <v>313</v>
       </c>
       <c r="CM32" s="18" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="CN32" s="18" t="s">
         <v>272</v>
@@ -12242,7 +12478,7 @@
         <v>232</v>
       </c>
       <c r="DG32" s="18" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="DH32" s="18" t="s">
         <v>267</v>
@@ -12252,7 +12488,7 @@
       </c>
     </row>
     <row r="33" spans="2:113" ht="22" x14ac:dyDescent="0.5">
-      <c r="B33" s="113" t="s">
+      <c r="B33" s="167" t="s">
         <v>6</v>
       </c>
       <c r="C33" s="12" t="s">
@@ -12324,13 +12560,13 @@
       <c r="Y33" s="18">
         <v>130</v>
       </c>
-      <c r="Z33" s="28" t="s">
-        <v>137</v>
-      </c>
-      <c r="AA33" s="28">
+      <c r="Z33" s="109" t="s">
+        <v>137</v>
+      </c>
+      <c r="AA33" s="145">
         <v>199</v>
       </c>
-      <c r="AB33" s="18">
+      <c r="AB33" s="127">
         <v>206.66666666666666</v>
       </c>
       <c r="AC33" s="18">
@@ -12590,7 +12826,7 @@
       </c>
     </row>
     <row r="34" spans="2:113" x14ac:dyDescent="0.5">
-      <c r="B34" s="113"/>
+      <c r="B34" s="167"/>
       <c r="C34" s="12" t="s">
         <v>24</v>
       </c>
@@ -12614,7 +12850,7 @@
         <v>291</v>
       </c>
       <c r="K34" s="18" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="L34" s="18" t="s">
         <v>137</v>
@@ -12650,7 +12886,7 @@
         <v>300</v>
       </c>
       <c r="W34" s="18" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="X34" s="18" t="s">
         <v>247</v>
@@ -12658,13 +12894,13 @@
       <c r="Y34" s="18" t="s">
         <v>157</v>
       </c>
-      <c r="Z34" s="28" t="s">
-        <v>137</v>
-      </c>
-      <c r="AA34" s="28" t="s">
-        <v>365</v>
-      </c>
-      <c r="AB34" s="18" t="s">
+      <c r="Z34" s="109" t="s">
+        <v>137</v>
+      </c>
+      <c r="AA34" s="145" t="s">
+        <v>363</v>
+      </c>
+      <c r="AB34" s="127" t="s">
         <v>248</v>
       </c>
       <c r="AC34" s="18" t="s">
@@ -12698,7 +12934,7 @@
         <v>297</v>
       </c>
       <c r="AM34" s="18" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="AN34" s="18" t="s">
         <v>137</v>
@@ -12770,7 +13006,7 @@
         <v>296</v>
       </c>
       <c r="BK34" s="28" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="BL34" s="18" t="s">
         <v>252</v>
@@ -12794,7 +13030,7 @@
         <v>285</v>
       </c>
       <c r="BS34" s="28" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="BT34" s="18" t="s">
         <v>165</v>
@@ -12818,7 +13054,7 @@
         <v>295</v>
       </c>
       <c r="CA34" s="18" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="CB34" s="18" t="s">
         <v>253</v>
@@ -12830,7 +13066,7 @@
         <v>273</v>
       </c>
       <c r="CE34" s="18" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="CF34" s="18" t="s">
         <v>137</v>
@@ -12854,7 +13090,7 @@
         <v>137</v>
       </c>
       <c r="CM34" s="28" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="CN34" s="18" t="s">
         <v>246</v>
@@ -12924,7 +13160,7 @@
       </c>
     </row>
     <row r="35" spans="2:113" ht="22" x14ac:dyDescent="0.5">
-      <c r="B35" s="113"/>
+      <c r="B35" s="167"/>
       <c r="C35" s="12" t="s">
         <v>26</v>
       </c>
@@ -12992,13 +13228,13 @@
       <c r="Y35" s="18">
         <v>130</v>
       </c>
-      <c r="Z35" s="18">
+      <c r="Z35" s="110">
         <v>190</v>
       </c>
-      <c r="AA35" s="18">
+      <c r="AA35" s="146">
         <v>199</v>
       </c>
-      <c r="AB35" s="18">
+      <c r="AB35" s="127">
         <v>270</v>
       </c>
       <c r="AC35" s="18">
@@ -13258,7 +13494,7 @@
       </c>
     </row>
     <row r="36" spans="2:113" x14ac:dyDescent="0.5">
-      <c r="B36" s="113"/>
+      <c r="B36" s="167"/>
       <c r="C36" s="12" t="s">
         <v>22</v>
       </c>
@@ -13318,7 +13554,7 @@
         <v>305</v>
       </c>
       <c r="W36" s="28" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="X36" s="18" t="s">
         <v>199</v>
@@ -13326,13 +13562,13 @@
       <c r="Y36" s="18" t="s">
         <v>171</v>
       </c>
-      <c r="Z36" s="18" t="s">
+      <c r="Z36" s="110" t="s">
         <v>302</v>
       </c>
-      <c r="AA36" s="18" t="s">
+      <c r="AA36" s="146" t="s">
         <v>286</v>
       </c>
-      <c r="AB36" s="18" t="s">
+      <c r="AB36" s="127" t="s">
         <v>165</v>
       </c>
       <c r="AC36" s="18" t="s">
@@ -13342,7 +13578,7 @@
         <v>303</v>
       </c>
       <c r="AE36" s="18" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="AF36" s="18" t="s">
         <v>199</v>
@@ -13414,7 +13650,7 @@
         <v>304</v>
       </c>
       <c r="BC36" s="28" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="BD36" s="18" t="s">
         <v>137</v>
@@ -13426,7 +13662,7 @@
         <v>305</v>
       </c>
       <c r="BG36" s="28" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="BH36" s="18" t="s">
         <v>259</v>
@@ -13486,7 +13722,7 @@
         <v>135</v>
       </c>
       <c r="CA36" s="18" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="CB36" s="18" t="s">
         <v>199</v>
@@ -13522,7 +13758,7 @@
         <v>137</v>
       </c>
       <c r="CM36" s="28" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="CN36" s="18" t="s">
         <v>259</v>
@@ -13582,7 +13818,7 @@
         <v>302</v>
       </c>
       <c r="DG36" s="18" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="DH36" s="18" t="s">
         <v>259</v>
@@ -13592,7 +13828,7 @@
       </c>
     </row>
     <row r="37" spans="2:113" ht="22" x14ac:dyDescent="0.5">
-      <c r="B37" s="113"/>
+      <c r="B37" s="167"/>
       <c r="C37" s="12" t="s">
         <v>27</v>
       </c>
@@ -13660,13 +13896,13 @@
       <c r="Y37" s="18">
         <v>130</v>
       </c>
-      <c r="Z37" s="18">
+      <c r="Z37" s="110">
         <v>190</v>
       </c>
-      <c r="AA37" s="18">
+      <c r="AA37" s="146">
         <v>199</v>
       </c>
-      <c r="AB37" s="18">
+      <c r="AB37" s="127">
         <v>255</v>
       </c>
       <c r="AC37" s="18">
@@ -13926,7 +14162,7 @@
       </c>
     </row>
     <row r="38" spans="2:113" x14ac:dyDescent="0.5">
-      <c r="B38" s="113"/>
+      <c r="B38" s="167"/>
       <c r="C38" s="12" t="s">
         <v>22</v>
       </c>
@@ -13950,7 +14186,7 @@
         <v>292</v>
       </c>
       <c r="K38" s="18" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="L38" s="18" t="s">
         <v>265</v>
@@ -13962,7 +14198,7 @@
         <v>307</v>
       </c>
       <c r="O38" s="18" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="P38" s="18" t="s">
         <v>266</v>
@@ -13974,7 +14210,7 @@
         <v>345</v>
       </c>
       <c r="S38" s="18" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="T38" s="18" t="s">
         <v>195</v>
@@ -13986,7 +14222,7 @@
         <v>307</v>
       </c>
       <c r="W38" s="18" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="X38" s="18" t="s">
         <v>200</v>
@@ -13994,13 +14230,13 @@
       <c r="Y38" s="18" t="s">
         <v>188</v>
       </c>
-      <c r="Z38" s="28" t="s">
+      <c r="Z38" s="109" t="s">
         <v>284</v>
       </c>
-      <c r="AA38" s="28" t="s">
-        <v>358</v>
-      </c>
-      <c r="AB38" s="18" t="s">
+      <c r="AA38" s="145" t="s">
+        <v>357</v>
+      </c>
+      <c r="AB38" s="127" t="s">
         <v>160</v>
       </c>
       <c r="AC38" s="18" t="s">
@@ -14034,7 +14270,7 @@
         <v>309</v>
       </c>
       <c r="AM38" s="18" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="AN38" s="18" t="s">
         <v>213</v>
@@ -14094,7 +14330,7 @@
         <v>292</v>
       </c>
       <c r="BG38" s="18" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="BH38" s="18" t="s">
         <v>267</v>
@@ -14106,7 +14342,7 @@
         <v>292</v>
       </c>
       <c r="BK38" s="18" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="BL38" s="18" t="s">
         <v>137</v>
@@ -14166,7 +14402,7 @@
         <v>312</v>
       </c>
       <c r="CE38" s="18" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="CF38" s="18" t="s">
         <v>271</v>
@@ -14188,7 +14424,7 @@
         <v>313</v>
       </c>
       <c r="CM38" s="18" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="CN38" s="18" t="s">
         <v>272</v>
@@ -14248,7 +14484,7 @@
         <v>232</v>
       </c>
       <c r="DG38" s="18" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="DH38" s="18" t="s">
         <v>267</v>
@@ -14331,14 +14567,14 @@
       <c r="Y39" s="2">
         <v>-10.25</v>
       </c>
-      <c r="Z39" s="2" t="str">
+      <c r="Z39" s="111" t="str">
         <f>IF(Z27&lt;&gt;"no data",IF(Z33&lt;&gt;"no data",IF(Z29&lt;&gt;"no data",IF(Z35&lt;&gt;"no data",(Z29+Z35)-(Z27+Z33),""),""),""),"")</f>
         <v/>
       </c>
-      <c r="AA39" s="2">
-        <v>0</v>
-      </c>
-      <c r="AB39" s="2">
+      <c r="AA39" s="147">
+        <v>0</v>
+      </c>
+      <c r="AB39" s="128">
         <v>190.5</v>
       </c>
       <c r="AC39" s="2">
@@ -14698,14 +14934,14 @@
       <c r="Y40" s="2">
         <v>-7.875</v>
       </c>
-      <c r="Z40" s="2">
+      <c r="Z40" s="111">
         <f>IF(Z29&lt;&gt;"no data",IF(Z37&lt;&gt;"no data",IF(Z31&lt;&gt;"no data",IF(Z35&lt;&gt;"no data",(Z31+Z37)-(Z29+Z35),""),""),""),"")</f>
         <v>-15.714290000000005</v>
       </c>
-      <c r="AA40" s="2">
-        <v>0</v>
-      </c>
-      <c r="AB40" s="2">
+      <c r="AA40" s="147">
+        <v>0</v>
+      </c>
+      <c r="AB40" s="128">
         <v>-45.5</v>
       </c>
       <c r="AC40" s="2">
@@ -15019,7 +15255,7 @@
         <f t="shared" ref="J41" si="8">IF(J40&lt;&gt;"",((J31+J37)-(J29+J35))/(J29+J35),"")</f>
         <v>-0.49734523433688255</v>
       </c>
-      <c r="K41" s="126">
+      <c r="K41" s="101">
         <v>-2.1000000000000001E-2</v>
       </c>
       <c r="L41" s="54">
@@ -15056,7 +15292,7 @@
         <f t="shared" ref="V41:CG41" si="9">IF(V40&lt;&gt;"",((V31+V37)-(V29+V35))/(V29+V35),"")</f>
         <v>2.9704048964218455</v>
       </c>
-      <c r="W41" s="126">
+      <c r="W41" s="101">
         <v>2.6890000000000001</v>
       </c>
       <c r="X41" s="54" t="e">
@@ -15067,14 +15303,14 @@
         <f t="shared" si="9"/>
         <v>#VALUE!</v>
       </c>
-      <c r="Z41" s="54">
+      <c r="Z41" s="112">
         <f t="shared" si="9"/>
         <v>-3.2069979591836745E-2</v>
       </c>
-      <c r="AA41" s="54">
-        <v>0</v>
-      </c>
-      <c r="AB41" s="54">
+      <c r="AA41" s="148">
+        <v>0</v>
+      </c>
+      <c r="AB41" s="129">
         <f t="shared" si="9"/>
         <v>-5.6138186304750155E-2</v>
       </c>
@@ -15086,7 +15322,7 @@
         <f t="shared" si="9"/>
         <v>-6.3074287494159789E-2</v>
       </c>
-      <c r="AE41" s="126">
+      <c r="AE41" s="101">
         <v>-7.4999999999999997E-2</v>
       </c>
       <c r="AF41" s="54">
@@ -15101,7 +15337,7 @@
         <f t="shared" si="9"/>
         <v>0.16640851589015748</v>
       </c>
-      <c r="AI41" s="126">
+      <c r="AI41" s="101">
         <v>-6.5000000000000002E-2</v>
       </c>
       <c r="AJ41" s="54">
@@ -15116,7 +15352,7 @@
         <f t="shared" si="9"/>
         <v>4.1457286432160803E-2</v>
       </c>
-      <c r="AM41" s="126">
+      <c r="AM41" s="101">
         <v>4.9000000000000002E-2</v>
       </c>
       <c r="AN41" s="54" t="e">
@@ -15131,7 +15367,7 @@
         <f>IF(AP40&lt;&gt;"",((AP31+AP37)-(3710+AP35))/(3710+AP35),"")</f>
         <v>4.0085934759733375E-3</v>
       </c>
-      <c r="AQ41" s="126">
+      <c r="AQ41" s="101">
         <v>-1.4999999999999999E-2</v>
       </c>
       <c r="AR41" s="54" t="str">
@@ -15394,10 +15630,10 @@
       </c>
     </row>
     <row r="42" spans="2:113" x14ac:dyDescent="0.5">
-      <c r="B42" s="114" t="s">
+      <c r="B42" s="168" t="s">
         <v>30</v>
       </c>
-      <c r="C42" s="114"/>
+      <c r="C42" s="168"/>
       <c r="D42" s="89">
         <f>Population_eurostat!C4</f>
         <v>8.7004710000000003</v>
@@ -15486,15 +15722,15 @@
         <f>Population_eurostat!D9</f>
         <v>10.610054999999999</v>
       </c>
-      <c r="Z42" s="89">
+      <c r="Z42" s="113">
         <f>Population_eurostat!E9</f>
         <v>10.693939</v>
       </c>
-      <c r="AA42" s="89">
+      <c r="AA42" s="149">
         <f>Population_eurostat!F9</f>
         <v>10.5</v>
       </c>
-      <c r="AB42" s="89">
+      <c r="AB42" s="130">
         <f>Population_eurostat!C10</f>
         <v>5.7072510000000003</v>
       </c>
@@ -15840,10 +16076,10 @@
       </c>
     </row>
     <row r="43" spans="2:113" x14ac:dyDescent="0.5">
-      <c r="B43" s="115" t="s">
+      <c r="B43" s="169" t="s">
         <v>31</v>
       </c>
-      <c r="C43" s="115"/>
+      <c r="C43" s="169"/>
       <c r="D43" s="33" t="s">
         <v>275</v>
       </c>
@@ -15918,15 +16154,15 @@
       <c r="Y43" s="33">
         <v>40.716094308653446</v>
       </c>
-      <c r="Z43" s="33" t="str">
+      <c r="Z43" s="114" t="str">
         <f>IF(((IF(OR(Z27="no data",Z27="n/a"),0,Z27))+IF(OR(Z33="no data",Z33="n/a"),0,Z33))&gt;0,((IF(OR(Z27="no data",Z27="n/a"),0,Z27))+IF(OR(Z33="no data",Z33="n/a"),0,Z33))/Z42,"")</f>
         <v/>
       </c>
-      <c r="AA43" s="33">
+      <c r="AA43" s="150">
         <f>IF(((IF(OR(AA27="no data",AA27="n/a"),0,AA27))+IF(OR(AA33="no data",AA33="n/a"),0,AA33))&gt;0,((IF(OR(AA27="no data",AA27="n/a"),0,AA27))+IF(OR(AA33="no data",AA33="n/a"),0,AA33))/AA42,"")</f>
         <v>49.904761904761905</v>
       </c>
-      <c r="AB43" s="33">
+      <c r="AB43" s="131">
         <v>108.63373627688706</v>
       </c>
       <c r="AC43" s="33">
@@ -16225,10 +16461,10 @@
       </c>
     </row>
     <row r="44" spans="2:113" x14ac:dyDescent="0.5">
-      <c r="B44" s="115" t="s">
+      <c r="B44" s="169" t="s">
         <v>32</v>
       </c>
-      <c r="C44" s="115"/>
+      <c r="C44" s="169"/>
       <c r="D44" s="33">
         <v>37.469235860909137</v>
       </c>
@@ -16305,15 +16541,15 @@
       <c r="Y44" s="33">
         <v>39.726467016429233</v>
       </c>
-      <c r="Z44" s="33">
+      <c r="Z44" s="114">
         <f>IF(((IF(OR(Z29="no data",Z29="n/a"),0,Z29))+IF(OR(Z35="no data",Z35="n/a"),0,Z35))&gt;0,((IF(OR(Z29="no data",Z29="n/a"),0,Z29))+IF(OR(Z35="no data",Z35="n/a"),0,Z35))/Z42,"")</f>
         <v>45.820347394912204</v>
       </c>
-      <c r="AA44" s="33">
+      <c r="AA44" s="150">
         <f>IF(((IF(OR(AA29="no data",AA29="n/a"),0,AA29))+IF(OR(AA35="no data",AA35="n/a"),0,AA35))&gt;0,((IF(OR(AA29="no data",AA29="n/a"),0,AA29))+IF(OR(AA35="no data",AA35="n/a"),0,AA35))/AA42,"")</f>
         <v>49.904761904761905</v>
       </c>
-      <c r="AB44" s="33">
+      <c r="AB44" s="131">
         <v>142.01232782647898</v>
       </c>
       <c r="AC44" s="33">
@@ -16612,10 +16848,10 @@
       </c>
     </row>
     <row r="45" spans="2:113" x14ac:dyDescent="0.5">
-      <c r="B45" s="115" t="s">
+      <c r="B45" s="169" t="s">
         <v>33</v>
       </c>
-      <c r="C45" s="115"/>
+      <c r="C45" s="169"/>
       <c r="D45" s="33">
         <v>35.917595725564745</v>
       </c>
@@ -16692,15 +16928,15 @@
       <c r="Y45" s="33">
         <v>38.984246547261066</v>
       </c>
-      <c r="Z45" s="33">
+      <c r="Z45" s="114">
         <f>IF(((IF(OR(Z31="no data",Z31="n/a"),0,Z31))+IF(OR(Z37="no data",Z37="n/a"),0,Z37))&gt;0,((IF(OR(Z31="no data",Z31="n/a"),0,Z31))+IF(OR(Z37="no data",Z37="n/a"),0,Z37))/Z42,"")</f>
         <v>44.3508897890665</v>
       </c>
-      <c r="AA45" s="33">
+      <c r="AA45" s="150">
         <f>IF(((IF(OR(AA31="no data",AA31="n/a"),0,AA31))+IF(OR(AA37="no data",AA37="n/a"),0,AA37))&gt;0,((IF(OR(AA31="no data",AA31="n/a"),0,AA31))+IF(OR(AA37="no data",AA37="n/a"),0,AA37))/AA42,"")</f>
         <v>49.904761904761905</v>
       </c>
-      <c r="AB45" s="33">
+      <c r="AB45" s="131">
         <v>134.04001330938485</v>
       </c>
       <c r="AC45" s="33">
@@ -17021,9 +17257,9 @@
       <c r="W46" s="1"/>
       <c r="X46" s="1"/>
       <c r="Y46" s="1"/>
-      <c r="Z46" s="1"/>
-      <c r="AA46" s="1"/>
-      <c r="AB46" s="1"/>
+      <c r="Z46" s="115"/>
+      <c r="AA46" s="151"/>
+      <c r="AB46" s="132"/>
       <c r="AC46" s="1"/>
       <c r="AD46" s="1"/>
       <c r="AE46" s="1"/>
@@ -17111,10 +17347,10 @@
       <c r="DI46" s="1"/>
     </row>
     <row r="47" spans="2:113" x14ac:dyDescent="0.5">
-      <c r="B47" s="112" t="s">
-        <v>0</v>
-      </c>
-      <c r="C47" s="112"/>
+      <c r="B47" s="166" t="s">
+        <v>0</v>
+      </c>
+      <c r="C47" s="166"/>
       <c r="D47" s="5">
         <f>D$3</f>
         <v>2016</v>
@@ -17203,15 +17439,15 @@
         <f t="shared" si="12"/>
         <v>2018</v>
       </c>
-      <c r="Z47" s="5">
+      <c r="Z47" s="107">
         <f t="shared" si="12"/>
         <v>2020</v>
       </c>
-      <c r="AA47" s="5">
+      <c r="AA47" s="143">
         <f t="shared" si="12"/>
         <v>2022</v>
       </c>
-      <c r="AB47" s="5">
+      <c r="AB47" s="125">
         <f t="shared" si="12"/>
         <v>2016</v>
       </c>
@@ -17557,10 +17793,10 @@
       </c>
     </row>
     <row r="48" spans="2:113" ht="20.350000000000001" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B48" s="117" t="s">
+      <c r="B48" s="171" t="s">
         <v>34</v>
       </c>
-      <c r="C48" s="117"/>
+      <c r="C48" s="171"/>
       <c r="D48" s="14"/>
       <c r="E48" s="14"/>
       <c r="F48" s="14"/>
@@ -17583,9 +17819,9 @@
       <c r="W48" s="14"/>
       <c r="X48" s="14"/>
       <c r="Y48" s="14"/>
-      <c r="Z48" s="14"/>
-      <c r="AA48" s="14"/>
-      <c r="AB48" s="14"/>
+      <c r="Z48" s="116"/>
+      <c r="AA48" s="152"/>
+      <c r="AB48" s="133"/>
       <c r="AC48" s="14"/>
       <c r="AD48" s="14"/>
       <c r="AE48" s="14"/>
@@ -17676,7 +17912,7 @@
       <c r="A49" t="s">
         <v>338</v>
       </c>
-      <c r="B49" s="118"/>
+      <c r="B49" s="172"/>
       <c r="C49" s="15" t="s">
         <v>35</v>
       </c>
@@ -17750,14 +17986,14 @@
       <c r="Y49" s="19">
         <v>15461192</v>
       </c>
-      <c r="Z49" s="19">
+      <c r="Z49" s="117">
         <f>'Feuil3-2020'!Y4</f>
         <v>14828588</v>
       </c>
-      <c r="AA49" s="19">
+      <c r="AA49" s="153">
         <v>14955989</v>
       </c>
-      <c r="AB49" s="19">
+      <c r="AB49" s="134">
         <v>11310855</v>
       </c>
       <c r="AC49" s="19">
@@ -18038,7 +18274,7 @@
       </c>
     </row>
     <row r="50" spans="1:211" ht="33" x14ac:dyDescent="0.5">
-      <c r="B50" s="119"/>
+      <c r="B50" s="173"/>
       <c r="C50" s="15" t="s">
         <v>36</v>
       </c>
@@ -18113,14 +18349,14 @@
       <c r="Y50" s="19">
         <v>15471234</v>
       </c>
-      <c r="Z50" s="19">
+      <c r="Z50" s="117">
         <f>'Feuil3-2020'!Y5</f>
         <v>14899862</v>
       </c>
-      <c r="AA50" s="19">
+      <c r="AA50" s="153">
         <v>15000000</v>
       </c>
-      <c r="AB50" s="19">
+      <c r="AB50" s="134">
         <v>11371338</v>
       </c>
       <c r="AC50" s="19">
@@ -18397,7 +18633,7 @@
       </c>
     </row>
     <row r="51" spans="1:211" ht="22" x14ac:dyDescent="0.5">
-      <c r="B51" s="119"/>
+      <c r="B51" s="173"/>
       <c r="C51" s="15" t="s">
         <v>37</v>
       </c>
@@ -18471,14 +18707,14 @@
       <c r="Y51" s="19">
         <v>9482202</v>
       </c>
-      <c r="Z51" s="19">
+      <c r="Z51" s="117">
         <f>'Feuil3-2020'!Y6</f>
         <v>9314302</v>
       </c>
-      <c r="AA51" s="19">
+      <c r="AA51" s="153">
         <v>9637280</v>
       </c>
-      <c r="AB51" s="19">
+      <c r="AB51" s="134">
         <v>11598945</v>
       </c>
       <c r="AC51" s="19">
@@ -18757,7 +18993,7 @@
       </c>
     </row>
     <row r="52" spans="1:211" ht="22" x14ac:dyDescent="0.5">
-      <c r="B52" s="119"/>
+      <c r="B52" s="173"/>
       <c r="C52" s="15" t="s">
         <v>38</v>
       </c>
@@ -18831,14 +19067,14 @@
       <c r="Y52" s="19">
         <v>503305</v>
       </c>
-      <c r="Z52" s="19">
+      <c r="Z52" s="117">
         <f>'Feuil3-2020'!Y7</f>
         <v>195501.55172641561</v>
       </c>
-      <c r="AA52" s="19">
+      <c r="AA52" s="153">
         <v>181319</v>
       </c>
-      <c r="AB52" s="19" t="s">
+      <c r="AB52" s="134" t="s">
         <v>137</v>
       </c>
       <c r="AC52" s="19">
@@ -19119,7 +19355,7 @@
     </row>
     <row r="53" spans="1:211" s="96" customFormat="1" ht="22" x14ac:dyDescent="0.5">
       <c r="A53" s="97"/>
-      <c r="B53" s="119"/>
+      <c r="B53" s="173"/>
       <c r="C53" s="98" t="s">
         <v>39</v>
       </c>
@@ -19194,14 +19430,14 @@
       <c r="Y53" s="99">
         <v>0</v>
       </c>
-      <c r="Z53" s="99">
+      <c r="Z53" s="118">
         <f>'Feuil3-2020'!Y8</f>
         <v>0</v>
       </c>
-      <c r="AA53" s="99">
+      <c r="AA53" s="154">
         <v>6935</v>
       </c>
-      <c r="AB53" s="99" t="s">
+      <c r="AB53" s="135" t="s">
         <v>137</v>
       </c>
       <c r="AC53" s="99">
@@ -19582,7 +19818,7 @@
       <c r="A54" t="s">
         <v>339</v>
       </c>
-      <c r="B54" s="119"/>
+      <c r="B54" s="173"/>
       <c r="C54" s="15" t="s">
         <v>40</v>
       </c>
@@ -19655,14 +19891,14 @@
       <c r="Y54" s="19">
         <v>9524430</v>
       </c>
-      <c r="Z54" s="19">
+      <c r="Z54" s="117">
         <f>'Feuil3-2020'!Y9</f>
         <v>9016813</v>
       </c>
-      <c r="AA54" s="19">
+      <c r="AA54" s="153">
         <v>9839685</v>
       </c>
-      <c r="AB54" s="19">
+      <c r="AB54" s="134">
         <v>7216809</v>
       </c>
       <c r="AC54" s="19">
@@ -20692,7 +20928,7 @@
       <c r="AD5" s="7"/>
     </row>
     <row r="6" spans="1:30" ht="22.85" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A6" s="109" t="s">
+      <c r="A6" s="163" t="s">
         <v>3</v>
       </c>
       <c r="B6" s="8" t="s">
@@ -20812,7 +21048,7 @@
       </c>
     </row>
     <row r="7" spans="1:30" ht="14.45" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A7" s="110"/>
+      <c r="A7" s="164"/>
       <c r="B7" s="8" t="s">
         <v>216</v>
       </c>
@@ -20930,7 +21166,7 @@
       </c>
     </row>
     <row r="8" spans="1:30" ht="14.45" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A8" s="111"/>
+      <c r="A8" s="165"/>
       <c r="B8" s="8" t="s">
         <v>5</v>
       </c>
@@ -21048,7 +21284,7 @@
       </c>
     </row>
     <row r="9" spans="1:30" ht="22.85" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A9" s="109" t="s">
+      <c r="A9" s="163" t="s">
         <v>6</v>
       </c>
       <c r="B9" s="8" t="s">
@@ -21168,7 +21404,7 @@
       </c>
     </row>
     <row r="10" spans="1:30" ht="14.45" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A10" s="110"/>
+      <c r="A10" s="164"/>
       <c r="B10" s="8" t="s">
         <v>216</v>
       </c>
@@ -21286,7 +21522,7 @@
       </c>
     </row>
     <row r="11" spans="1:30" ht="14.45" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A11" s="111"/>
+      <c r="A11" s="165"/>
       <c r="B11" s="8" t="s">
         <v>5</v>
       </c>
@@ -21404,10 +21640,10 @@
       </c>
     </row>
     <row r="12" spans="1:30" ht="14.45" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A12" s="123" t="s">
+      <c r="A12" s="177" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="124"/>
+      <c r="B12" s="178"/>
       <c r="C12" s="21">
         <f>article_17_synthesis_table!F12</f>
         <v>0</v>
@@ -21522,10 +21758,10 @@
       </c>
     </row>
     <row r="13" spans="1:30" ht="14.45" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A13" s="123" t="s">
+      <c r="A13" s="177" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="124"/>
+      <c r="B13" s="178"/>
       <c r="C13" s="17" t="str">
         <f>article_17_synthesis_table!F13</f>
         <v>no data</v>
@@ -21674,7 +21910,7 @@
       <c r="AD14" s="7"/>
     </row>
     <row r="15" spans="1:30" ht="22.85" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A15" s="109" t="s">
+      <c r="A15" s="163" t="s">
         <v>3</v>
       </c>
       <c r="B15" s="8" t="s">
@@ -21794,7 +22030,7 @@
       </c>
     </row>
     <row r="16" spans="1:30" ht="22.85" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A16" s="111"/>
+      <c r="A16" s="165"/>
       <c r="B16" s="8" t="s">
         <v>12</v>
       </c>
@@ -21912,7 +22148,7 @@
       </c>
     </row>
     <row r="17" spans="1:30" ht="22.85" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A17" s="109" t="s">
+      <c r="A17" s="163" t="s">
         <v>6</v>
       </c>
       <c r="B17" s="8" t="s">
@@ -22032,7 +22268,7 @@
       </c>
     </row>
     <row r="18" spans="1:30" ht="22.85" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A18" s="111"/>
+      <c r="A18" s="165"/>
       <c r="B18" s="8" t="s">
         <v>14</v>
       </c>
@@ -22184,7 +22420,7 @@
       <c r="AD19" s="7"/>
     </row>
     <row r="20" spans="1:30" ht="22.85" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A20" s="109" t="s">
+      <c r="A20" s="163" t="s">
         <v>3</v>
       </c>
       <c r="B20" s="8" t="s">
@@ -22304,7 +22540,7 @@
       </c>
     </row>
     <row r="21" spans="1:30" ht="22.85" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A21" s="111"/>
+      <c r="A21" s="165"/>
       <c r="B21" s="8" t="s">
         <v>17</v>
       </c>
@@ -22422,7 +22658,7 @@
       </c>
     </row>
     <row r="22" spans="1:30" ht="22.85" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A22" s="109" t="s">
+      <c r="A22" s="163" t="s">
         <v>6</v>
       </c>
       <c r="B22" s="8" t="s">
@@ -22542,7 +22778,7 @@
       </c>
     </row>
     <row r="23" spans="1:30" ht="14.45" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A23" s="111"/>
+      <c r="A23" s="165"/>
       <c r="B23" s="8" t="s">
         <v>19</v>
       </c>
@@ -22785,7 +23021,7 @@
       <c r="AD26" s="11"/>
     </row>
     <row r="27" spans="1:30" ht="22.85" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A27" s="120" t="s">
+      <c r="A27" s="174" t="s">
         <v>3</v>
       </c>
       <c r="B27" s="12" t="s">
@@ -22905,7 +23141,7 @@
       </c>
     </row>
     <row r="28" spans="1:30" ht="14.45" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A28" s="121"/>
+      <c r="A28" s="175"/>
       <c r="B28" s="12" t="s">
         <v>22</v>
       </c>
@@ -23023,7 +23259,7 @@
       </c>
     </row>
     <row r="29" spans="1:30" ht="22.85" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A29" s="121"/>
+      <c r="A29" s="175"/>
       <c r="B29" s="12" t="s">
         <v>23</v>
       </c>
@@ -23141,7 +23377,7 @@
       </c>
     </row>
     <row r="30" spans="1:30" ht="14.45" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A30" s="121"/>
+      <c r="A30" s="175"/>
       <c r="B30" s="12" t="s">
         <v>24</v>
       </c>
@@ -23259,7 +23495,7 @@
       </c>
     </row>
     <row r="31" spans="1:30" ht="22.85" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A31" s="121"/>
+      <c r="A31" s="175"/>
       <c r="B31" s="12" t="s">
         <v>25</v>
       </c>
@@ -23377,7 +23613,7 @@
       </c>
     </row>
     <row r="32" spans="1:30" ht="14.45" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A32" s="122"/>
+      <c r="A32" s="176"/>
       <c r="B32" s="12" t="s">
         <v>22</v>
       </c>
@@ -23495,7 +23731,7 @@
       </c>
     </row>
     <row r="33" spans="1:30" ht="22.85" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A33" s="120" t="s">
+      <c r="A33" s="174" t="s">
         <v>6</v>
       </c>
       <c r="B33" s="12" t="s">
@@ -23615,7 +23851,7 @@
       </c>
     </row>
     <row r="34" spans="1:30" ht="14.45" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A34" s="121"/>
+      <c r="A34" s="175"/>
       <c r="B34" s="12" t="s">
         <v>24</v>
       </c>
@@ -23733,7 +23969,7 @@
       </c>
     </row>
     <row r="35" spans="1:30" ht="22.85" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A35" s="121"/>
+      <c r="A35" s="175"/>
       <c r="B35" s="12" t="s">
         <v>26</v>
       </c>
@@ -23851,7 +24087,7 @@
       </c>
     </row>
     <row r="36" spans="1:30" ht="14.45" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A36" s="121"/>
+      <c r="A36" s="175"/>
       <c r="B36" s="12" t="s">
         <v>22</v>
       </c>
@@ -23969,7 +24205,7 @@
       </c>
     </row>
     <row r="37" spans="1:30" ht="22" x14ac:dyDescent="0.5">
-      <c r="A37" s="121"/>
+      <c r="A37" s="175"/>
       <c r="B37" s="12" t="s">
         <v>27</v>
       </c>
@@ -24087,7 +24323,7 @@
       </c>
     </row>
     <row r="38" spans="1:30" x14ac:dyDescent="0.5">
-      <c r="A38" s="122"/>
+      <c r="A38" s="176"/>
       <c r="B38" s="12" t="s">
         <v>22</v>
       </c>
@@ -24559,10 +24795,10 @@
       </c>
     </row>
     <row r="42" spans="1:30" x14ac:dyDescent="0.5">
-      <c r="A42" s="114" t="s">
+      <c r="A42" s="168" t="s">
         <v>30</v>
       </c>
-      <c r="B42" s="114"/>
+      <c r="B42" s="168"/>
       <c r="C42" s="20">
         <f>article_17_synthesis_table!F42</f>
         <v>8.9010639999999999</v>
@@ -24677,10 +24913,10 @@
       </c>
     </row>
     <row r="43" spans="1:30" x14ac:dyDescent="0.5">
-      <c r="A43" s="115" t="s">
+      <c r="A43" s="169" t="s">
         <v>31</v>
       </c>
-      <c r="B43" s="115"/>
+      <c r="B43" s="169"/>
       <c r="C43" s="33" t="str">
         <f>article_17_synthesis_table!F43</f>
         <v/>
@@ -24795,10 +25031,10 @@
       </c>
     </row>
     <row r="44" spans="1:30" x14ac:dyDescent="0.5">
-      <c r="A44" s="115" t="s">
+      <c r="A44" s="169" t="s">
         <v>32</v>
       </c>
-      <c r="B44" s="115"/>
+      <c r="B44" s="169"/>
       <c r="C44" s="33">
         <f>article_17_synthesis_table!F44</f>
         <v>24.716146294420533</v>
@@ -24913,10 +25149,10 @@
       </c>
     </row>
     <row r="45" spans="1:30" x14ac:dyDescent="0.5">
-      <c r="A45" s="115" t="s">
+      <c r="A45" s="169" t="s">
         <v>33</v>
       </c>
-      <c r="B45" s="115"/>
+      <c r="B45" s="169"/>
       <c r="C45" s="33">
         <f>article_17_synthesis_table!F45</f>
         <v>30.221106150905104</v>
@@ -25031,10 +25267,10 @@
       </c>
     </row>
     <row r="47" spans="1:30" x14ac:dyDescent="0.5">
-      <c r="A47" s="112" t="s">
-        <v>0</v>
-      </c>
-      <c r="B47" s="112"/>
+      <c r="A47" s="166" t="s">
+        <v>0</v>
+      </c>
+      <c r="B47" s="166"/>
       <c r="C47" s="5">
         <v>2020</v>
       </c>
@@ -25121,10 +25357,10 @@
       </c>
     </row>
     <row r="48" spans="1:30" x14ac:dyDescent="0.5">
-      <c r="A48" s="117" t="s">
+      <c r="A48" s="171" t="s">
         <v>34</v>
       </c>
-      <c r="B48" s="117"/>
+      <c r="B48" s="171"/>
       <c r="C48" s="14"/>
       <c r="D48" s="14"/>
       <c r="E48" s="14"/>
@@ -25155,7 +25391,7 @@
       <c r="AD48" s="14"/>
     </row>
     <row r="49" spans="1:30" x14ac:dyDescent="0.5">
-      <c r="A49" s="118"/>
+      <c r="A49" s="172"/>
       <c r="B49" s="15" t="s">
         <v>35</v>
       </c>
@@ -25273,7 +25509,7 @@
       </c>
     </row>
     <row r="50" spans="1:30" ht="22" x14ac:dyDescent="0.5">
-      <c r="A50" s="119"/>
+      <c r="A50" s="173"/>
       <c r="B50" s="15" t="s">
         <v>36</v>
       </c>
@@ -25391,7 +25627,7 @@
       </c>
     </row>
     <row r="51" spans="1:30" ht="22" x14ac:dyDescent="0.5">
-      <c r="A51" s="119"/>
+      <c r="A51" s="173"/>
       <c r="B51" s="15" t="s">
         <v>37</v>
       </c>
@@ -25509,7 +25745,7 @@
       </c>
     </row>
     <row r="52" spans="1:30" ht="22" x14ac:dyDescent="0.5">
-      <c r="A52" s="119"/>
+      <c r="A52" s="173"/>
       <c r="B52" s="15" t="s">
         <v>38</v>
       </c>
@@ -25627,7 +25863,7 @@
       </c>
     </row>
     <row r="53" spans="1:30" ht="22" x14ac:dyDescent="0.5">
-      <c r="A53" s="119"/>
+      <c r="A53" s="173"/>
       <c r="B53" s="15" t="s">
         <v>39</v>
       </c>
@@ -25745,7 +25981,7 @@
       </c>
     </row>
     <row r="54" spans="1:30" ht="22" x14ac:dyDescent="0.5">
-      <c r="A54" s="119"/>
+      <c r="A54" s="173"/>
       <c r="B54" s="15" t="s">
         <v>40</v>
       </c>
@@ -26642,10 +26878,10 @@
       </c>
     </row>
     <row r="3" spans="2:114" x14ac:dyDescent="0.5">
-      <c r="B3" s="112" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="112"/>
+      <c r="B3" s="166" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="166"/>
       <c r="D3" s="4">
         <v>2014</v>
       </c>
@@ -27215,7 +27451,7 @@
       <c r="DJ5" s="7"/>
     </row>
     <row r="6" spans="2:114" ht="22.85" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B6" s="104" t="s">
+      <c r="B6" s="158" t="s">
         <v>3</v>
       </c>
       <c r="C6" s="8" t="s">
@@ -27556,7 +27792,7 @@
       </c>
     </row>
     <row r="7" spans="2:114" ht="14.45" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B7" s="104"/>
+      <c r="B7" s="158"/>
       <c r="C7" s="8" t="s">
         <v>216</v>
       </c>
@@ -27895,7 +28131,7 @@
       </c>
     </row>
     <row r="8" spans="2:114" ht="14.45" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B8" s="104"/>
+      <c r="B8" s="158"/>
       <c r="C8" s="8" t="s">
         <v>5</v>
       </c>
@@ -28234,7 +28470,7 @@
       </c>
     </row>
     <row r="9" spans="2:114" ht="22.85" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B9" s="109" t="s">
+      <c r="B9" s="163" t="s">
         <v>6</v>
       </c>
       <c r="C9" s="8" t="s">
@@ -28575,7 +28811,7 @@
       </c>
     </row>
     <row r="10" spans="2:114" ht="13.85" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B10" s="110"/>
+      <c r="B10" s="164"/>
       <c r="C10" s="8" t="s">
         <v>216</v>
       </c>
@@ -28914,7 +29150,7 @@
       </c>
     </row>
     <row r="11" spans="2:114" ht="14.45" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B11" s="111"/>
+      <c r="B11" s="165"/>
       <c r="C11" s="8" t="s">
         <v>5</v>
       </c>
@@ -29253,10 +29489,10 @@
       </c>
     </row>
     <row r="12" spans="2:114" ht="14.45" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B12" s="107" t="s">
+      <c r="B12" s="161" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="108"/>
+      <c r="C12" s="162"/>
       <c r="D12" s="21">
         <f>IF(D6="n/a",0,IF(D6="no data",0,D6))+IF(D9="n/a",0,IF(D9="no data",0,D9))</f>
         <v>0</v>
@@ -29703,10 +29939,10 @@
       </c>
     </row>
     <row r="13" spans="2:114" ht="14.45" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B13" s="107" t="s">
+      <c r="B13" s="161" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="108"/>
+      <c r="C13" s="162"/>
       <c r="D13" s="9" t="s">
         <v>139</v>
       </c>
@@ -30159,7 +30395,7 @@
       <c r="DJ14" s="7"/>
     </row>
     <row r="15" spans="2:114" ht="22.85" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B15" s="104" t="s">
+      <c r="B15" s="158" t="s">
         <v>3</v>
       </c>
       <c r="C15" s="8" t="s">
@@ -30500,7 +30736,7 @@
       </c>
     </row>
     <row r="16" spans="2:114" ht="22.85" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B16" s="104"/>
+      <c r="B16" s="158"/>
       <c r="C16" s="8" t="s">
         <v>12</v>
       </c>
@@ -30839,7 +31075,7 @@
       </c>
     </row>
     <row r="17" spans="2:114" ht="22.85" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B17" s="104" t="s">
+      <c r="B17" s="158" t="s">
         <v>6</v>
       </c>
       <c r="C17" s="8" t="s">
@@ -31180,7 +31416,7 @@
       </c>
     </row>
     <row r="18" spans="2:114" ht="22.85" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B18" s="104"/>
+      <c r="B18" s="158"/>
       <c r="C18" s="8" t="s">
         <v>14</v>
       </c>
@@ -31636,7 +31872,7 @@
       <c r="DJ19" s="7"/>
     </row>
     <row r="20" spans="2:114" ht="22" x14ac:dyDescent="0.5">
-      <c r="B20" s="104" t="s">
+      <c r="B20" s="158" t="s">
         <v>3</v>
       </c>
       <c r="C20" s="8" t="s">
@@ -32006,7 +32242,7 @@
       </c>
     </row>
     <row r="21" spans="2:114" ht="22" x14ac:dyDescent="0.5">
-      <c r="B21" s="104"/>
+      <c r="B21" s="158"/>
       <c r="C21" s="8" t="s">
         <v>17</v>
       </c>
@@ -32456,7 +32692,7 @@
       </c>
     </row>
     <row r="22" spans="2:114" ht="22" x14ac:dyDescent="0.5">
-      <c r="B22" s="105" t="s">
+      <c r="B22" s="159" t="s">
         <v>6</v>
       </c>
       <c r="C22" s="8" t="s">
@@ -32797,7 +33033,7 @@
       </c>
     </row>
     <row r="23" spans="2:114" x14ac:dyDescent="0.5">
-      <c r="B23" s="105"/>
+      <c r="B23" s="159"/>
       <c r="C23" s="8" t="s">
         <v>19</v>
       </c>
@@ -33136,10 +33372,10 @@
       </c>
     </row>
     <row r="25" spans="2:114" x14ac:dyDescent="0.5">
-      <c r="B25" s="112" t="s">
-        <v>0</v>
-      </c>
-      <c r="C25" s="112"/>
+      <c r="B25" s="166" t="s">
+        <v>0</v>
+      </c>
+      <c r="C25" s="166"/>
       <c r="D25" s="4">
         <v>2014</v>
       </c>
@@ -33475,10 +33711,10 @@
       </c>
     </row>
     <row r="26" spans="2:114" x14ac:dyDescent="0.5">
-      <c r="B26" s="125" t="s">
+      <c r="B26" s="179" t="s">
         <v>20</v>
       </c>
-      <c r="C26" s="125"/>
+      <c r="C26" s="179"/>
       <c r="D26" s="11"/>
       <c r="E26" s="11"/>
       <c r="F26" s="11"/>
@@ -33592,7 +33828,7 @@
       <c r="DJ26" s="11"/>
     </row>
     <row r="27" spans="2:114" ht="22" x14ac:dyDescent="0.5">
-      <c r="B27" s="113" t="s">
+      <c r="B27" s="167" t="s">
         <v>3</v>
       </c>
       <c r="C27" s="12" t="s">
@@ -33933,7 +34169,7 @@
       </c>
     </row>
     <row r="28" spans="2:114" x14ac:dyDescent="0.5">
-      <c r="B28" s="113"/>
+      <c r="B28" s="167"/>
       <c r="C28" s="12" t="s">
         <v>22</v>
       </c>
@@ -34270,7 +34506,7 @@
       </c>
     </row>
     <row r="29" spans="2:114" ht="22" x14ac:dyDescent="0.5">
-      <c r="B29" s="113"/>
+      <c r="B29" s="167"/>
       <c r="C29" s="12" t="s">
         <v>23</v>
       </c>
@@ -34607,7 +34843,7 @@
       </c>
     </row>
     <row r="30" spans="2:114" x14ac:dyDescent="0.5">
-      <c r="B30" s="113"/>
+      <c r="B30" s="167"/>
       <c r="C30" s="12" t="s">
         <v>24</v>
       </c>
@@ -34944,7 +35180,7 @@
       </c>
     </row>
     <row r="31" spans="2:114" ht="22" x14ac:dyDescent="0.5">
-      <c r="B31" s="113"/>
+      <c r="B31" s="167"/>
       <c r="C31" s="12" t="s">
         <v>25</v>
       </c>
@@ -35281,7 +35517,7 @@
       </c>
     </row>
     <row r="32" spans="2:114" x14ac:dyDescent="0.5">
-      <c r="B32" s="113"/>
+      <c r="B32" s="167"/>
       <c r="C32" s="12" t="s">
         <v>22</v>
       </c>
@@ -35618,7 +35854,7 @@
       </c>
     </row>
     <row r="33" spans="2:114" ht="22" x14ac:dyDescent="0.5">
-      <c r="B33" s="113" t="s">
+      <c r="B33" s="167" t="s">
         <v>6</v>
       </c>
       <c r="C33" s="12" t="s">
@@ -35959,7 +36195,7 @@
       </c>
     </row>
     <row r="34" spans="2:114" x14ac:dyDescent="0.5">
-      <c r="B34" s="113"/>
+      <c r="B34" s="167"/>
       <c r="C34" s="12" t="s">
         <v>24</v>
       </c>
@@ -36296,7 +36532,7 @@
       </c>
     </row>
     <row r="35" spans="2:114" ht="22" x14ac:dyDescent="0.5">
-      <c r="B35" s="113"/>
+      <c r="B35" s="167"/>
       <c r="C35" s="12" t="s">
         <v>26</v>
       </c>
@@ -36633,7 +36869,7 @@
       </c>
     </row>
     <row r="36" spans="2:114" x14ac:dyDescent="0.5">
-      <c r="B36" s="113"/>
+      <c r="B36" s="167"/>
       <c r="C36" s="12" t="s">
         <v>22</v>
       </c>
@@ -36970,7 +37206,7 @@
       </c>
     </row>
     <row r="37" spans="2:114" ht="22" x14ac:dyDescent="0.5">
-      <c r="B37" s="113"/>
+      <c r="B37" s="167"/>
       <c r="C37" s="12" t="s">
         <v>27</v>
       </c>
@@ -37307,7 +37543,7 @@
       </c>
     </row>
     <row r="38" spans="2:114" x14ac:dyDescent="0.5">
-      <c r="B38" s="113"/>
+      <c r="B38" s="167"/>
       <c r="C38" s="12" t="s">
         <v>22</v>
       </c>
@@ -38804,10 +39040,10 @@
       </c>
     </row>
     <row r="42" spans="2:114" x14ac:dyDescent="0.5">
-      <c r="B42" s="114" t="s">
+      <c r="B42" s="168" t="s">
         <v>30</v>
       </c>
-      <c r="C42" s="114"/>
+      <c r="C42" s="168"/>
       <c r="D42" s="22">
         <v>8.5077859999999994</v>
       </c>
@@ -39170,10 +39406,10 @@
       </c>
     </row>
     <row r="43" spans="2:114" x14ac:dyDescent="0.5">
-      <c r="B43" s="115" t="s">
+      <c r="B43" s="169" t="s">
         <v>31</v>
       </c>
-      <c r="C43" s="115"/>
+      <c r="C43" s="169"/>
       <c r="D43" s="33">
         <v>36.202132963852172</v>
       </c>
@@ -39536,10 +39772,10 @@
       </c>
     </row>
     <row r="44" spans="2:114" x14ac:dyDescent="0.5">
-      <c r="B44" s="115" t="s">
+      <c r="B44" s="169" t="s">
         <v>32</v>
       </c>
-      <c r="C44" s="115"/>
+      <c r="C44" s="169"/>
       <c r="D44" s="33">
         <v>38.67046021138755</v>
       </c>
@@ -39902,10 +40138,10 @@
       </c>
     </row>
     <row r="45" spans="2:114" x14ac:dyDescent="0.5">
-      <c r="B45" s="115" t="s">
+      <c r="B45" s="169" t="s">
         <v>33</v>
       </c>
-      <c r="C45" s="115"/>
+      <c r="C45" s="169"/>
       <c r="D45" s="33">
         <v>39.258157175086446</v>
       </c>
@@ -40603,10 +40839,10 @@
       </c>
     </row>
     <row r="47" spans="2:114" x14ac:dyDescent="0.5">
-      <c r="B47" s="112" t="s">
-        <v>0</v>
-      </c>
-      <c r="C47" s="112"/>
+      <c r="B47" s="166" t="s">
+        <v>0</v>
+      </c>
+      <c r="C47" s="166"/>
       <c r="D47" s="4">
         <v>2014</v>
       </c>
@@ -40942,10 +41178,10 @@
       </c>
     </row>
     <row r="48" spans="2:114" x14ac:dyDescent="0.5">
-      <c r="B48" s="117" t="s">
+      <c r="B48" s="171" t="s">
         <v>34</v>
       </c>
-      <c r="C48" s="117"/>
+      <c r="C48" s="171"/>
       <c r="D48" s="14"/>
       <c r="E48" s="14"/>
       <c r="F48" s="14"/>
@@ -41062,7 +41298,7 @@
       <c r="A49" t="s">
         <v>338</v>
       </c>
-      <c r="B49" s="118"/>
+      <c r="B49" s="172"/>
       <c r="C49" s="15" t="s">
         <v>35</v>
       </c>
@@ -41428,7 +41664,7 @@
       </c>
     </row>
     <row r="50" spans="1:114" ht="33" x14ac:dyDescent="0.5">
-      <c r="B50" s="119"/>
+      <c r="B50" s="173"/>
       <c r="C50" s="15" t="s">
         <v>36</v>
       </c>
@@ -41788,7 +42024,7 @@
       </c>
     </row>
     <row r="51" spans="1:114" ht="22" x14ac:dyDescent="0.5">
-      <c r="B51" s="119"/>
+      <c r="B51" s="173"/>
       <c r="C51" s="15" t="s">
         <v>37</v>
       </c>
@@ -42154,7 +42390,7 @@
       </c>
     </row>
     <row r="52" spans="1:114" ht="22" x14ac:dyDescent="0.5">
-      <c r="B52" s="119"/>
+      <c r="B52" s="173"/>
       <c r="C52" s="15" t="s">
         <v>38</v>
       </c>
@@ -42520,7 +42756,7 @@
       </c>
     </row>
     <row r="53" spans="1:114" ht="22" x14ac:dyDescent="0.5">
-      <c r="B53" s="119"/>
+      <c r="B53" s="173"/>
       <c r="C53" s="15" t="s">
         <v>39</v>
       </c>
@@ -42889,7 +43125,7 @@
       <c r="A54" t="s">
         <v>339</v>
       </c>
-      <c r="B54" s="119"/>
+      <c r="B54" s="173"/>
       <c r="C54" s="15" t="s">
         <v>40</v>
       </c>

</xml_diff>